<commit_message>
Borro title del dataset "Internos del SPF"
</commit_message>
<xml_diff>
--- a/tests/samples/catalogo_justicia.xlsx
+++ b/tests/samples/catalogo_justicia.xlsx
@@ -1,17 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="124226"/>
+  <bookViews>
+    <workbookView xWindow="270" yWindow="525" windowWidth="23415" windowHeight="9405" activeTab="2"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Catalog" sheetId="1" r:id="rId3"/>
-    <sheet state="visible" name="Theme" sheetId="2" r:id="rId4"/>
-    <sheet state="visible" name="Dataset" sheetId="3" r:id="rId5"/>
-    <sheet state="visible" name="Distribution" sheetId="4" r:id="rId6"/>
-    <sheet state="visible" name="Field" sheetId="5" r:id="rId7"/>
-    <sheet state="visible" name="Notas y referencias" sheetId="6" r:id="rId8"/>
+    <sheet name="Catalog" sheetId="1" r:id="rId1"/>
+    <sheet name="Theme" sheetId="2" r:id="rId2"/>
+    <sheet name="Dataset" sheetId="3" r:id="rId3"/>
+    <sheet name="Distribution" sheetId="4" r:id="rId4"/>
+    <sheet name="Field" sheetId="5" r:id="rId5"/>
+    <sheet name="Notas y referencias" sheetId="6" r:id="rId6"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -21,12 +24,19 @@
     <author/>
   </authors>
   <commentList>
-    <comment authorId="0" ref="A1">
+    <comment ref="A1" authorId="0">
       <text>
-        <t xml:space="preserve">Dado que siempre habrá exactamente una entrada por cada uno de los campos propios de catálogo: ¿no mejora la legibilidad de *esta* worksheet transponerla (es decir, que los nombre de campos estén en la primer *columna*, en lugar de la primera *fila*?
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Dado que siempre habrá exactamente una entrada por cada uno de los campos propios de catálogo: ¿no mejora la legibilidad de *esta* worksheet transponerla (es decir, que los nombre de campos estén en la primer *columna*, en lugar de la primera *fila*?
 	-Gonzalo Barrera Borla
 Entiendo que te referis a esta hoja Catalog. Personalmente la dejaría asi, para que quede igual que las otras hojas y con la intencion de  "hacerla mas simple de completar" para  organismos.
 	-Fernando Petrone</t>
+        </r>
       </text>
     </comment>
   </commentList>
@@ -39,10 +49,17 @@
     <author/>
   </authors>
   <commentList>
-    <comment authorId="0" ref="Q2">
+    <comment ref="Q2" authorId="0">
       <text>
-        <t xml:space="preserve">la api tiene "name"="base-de-datos-legislativos-infoleg". Eso mas la homepage conformaría la landingPage + "/dataset/"
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>la api tiene "name"="base-de-datos-legislativos-infoleg". Eso mas la homepage conformaría la landingPage + "/dataset/"
 	-Fernando Petrone</t>
+        </r>
       </text>
     </comment>
   </commentList>
@@ -55,16 +72,30 @@
     <author/>
   </authors>
   <commentList>
-    <comment authorId="0" ref="A1">
+    <comment ref="A1" authorId="0">
       <text>
-        <t xml:space="preserve">este campo sale en la metadata de las distribuciones de la api de ckan
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>este campo sale en la metadata de las distribuciones de la api de ckan
 	-Fernando Petrone</t>
+        </r>
       </text>
     </comment>
-    <comment authorId="0" ref="C2">
+    <comment ref="C2" authorId="0">
       <text>
-        <t xml:space="preserve">en la API tenemos id ="8db246a2-48dd-4f2f-b08e-ab6293747882". Si le agregamos al inicio el valor de dataset:landingPage + "/archivo/"; obtendremos la accessURL
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>en la API tenemos id ="8db246a2-48dd-4f2f-b08e-ab6293747882". Si le agregamos al inicio el valor de dataset:landingPage + "/archivo/"; obtendremos la accessURL
 	-Fernando Petrone</t>
+        </r>
       </text>
     </comment>
   </commentList>
@@ -77,30 +108,58 @@
     <author/>
   </authors>
   <commentList>
-    <comment authorId="0" ref="B1">
+    <comment ref="B1" authorId="0">
       <text>
-        <t xml:space="preserve">no sé como sería el "ciclo de vida" de la planilla pero el cambio de titulo de la dist podría traer problemas, que en principio serían pocos y se resolverían "a mano". Entiendo que hablamos esto, pero lo marco por las dudas +agusbenassi@gmail.com
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>no sé como sería el "ciclo de vida" de la planilla pero el cambio de titulo de la dist podría traer problemas, que en principio serían pocos y se resolverían "a mano". Entiendo que hablamos esto, pero lo marco por las dudas +agusbenassi@gmail.com
 	-Fernando Petrone
 hacés bien en remarcarlo. El efecto que tendría el cambio de nombre es sumar una "nueva distribución" y "destruir una distribución que ya no está", según entiendo yo. Pero creo que lo veremos bien cuando hagamos pruebas
 	-Agustín Benassi</t>
+        </r>
       </text>
     </comment>
-    <comment authorId="0" ref="D50">
+    <comment ref="D4" authorId="0">
       <text>
-        <t xml:space="preserve">string poruqe tiene barra que separa num y año
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>string porque incluye algunos campos "S/N"
 	-Fernando Petrone</t>
+        </r>
       </text>
     </comment>
-    <comment authorId="0" ref="D8">
+    <comment ref="D8" authorId="0">
       <text>
-        <t xml:space="preserve">Que hacemos en estos casos? El formato en el csv es "10/06/2013", en la ISO  (YYYY-MM-DD)
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Que hacemos en estos casos? El formato en el csv es "10/06/2013", en la ISO  (YYYY-MM-DD)
 	-Fernando Petrone</t>
+        </r>
       </text>
     </comment>
-    <comment authorId="0" ref="D4">
+    <comment ref="D50" authorId="0">
       <text>
-        <t xml:space="preserve">string porque incluye algunos campos "S/N"
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>string poruqe tiene barra que separa num y año
 	-Fernando Petrone</t>
+        </r>
       </text>
     </comment>
   </commentList>
@@ -108,7 +167,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1099" uniqueCount="645">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1098" uniqueCount="645">
   <si>
     <t>theme_id</t>
   </si>
@@ -230,8 +289,7 @@
     <t>Sistema penitenciario</t>
   </si>
   <si>
-    <t>Portal de Datos de Justicia de la República Argentina. El Portal publica datos del sistema de justicia de modo que pueda ser reutilizada para efectuar visualizaciones o desarrollo de aplicaciones. Esta herramienta se propone como un punto de encuentro entre las organizaciones de justicia y la ciudadanía.
-</t>
+    <t>Portal de Datos de Justicia de la República Argentina. El Portal publica datos del sistema de justicia de modo que pueda ser reutilizada para efectuar visualizaciones o desarrollo de aplicaciones. Esta herramienta se propone como un punto de encuentro entre las organizaciones de justicia y la ciudadanía.</t>
   </si>
   <si>
     <t>Datasets referidos al sistema penitenciario</t>
@@ -315,8 +373,7 @@
     <t>datosabiertos@saij.gob.ar</t>
   </si>
   <si>
-    <t>datosabiertos@saij.gob.ar
-</t>
+    <t>datosabiertos@saij.gob.ar</t>
   </si>
   <si>
     <t>http://datos.gob.ar/superThemeTaxonomy.json</t>
@@ -325,15 +382,13 @@
     <t>JUST</t>
   </si>
   <si>
-    <t>
-acordadas,boletín oficial,decisiones ,administrativas,decretos,disposiciones,leyes,resoluciones</t>
+    <t>acordadas,boletín oficial,decisiones ,administrativas,decretos,disposiciones,leyes,resoluciones</t>
   </si>
   <si>
     <t>R/P1M</t>
   </si>
   <si>
-    <t>2016-09-05T18:25:21.249967
-</t>
+    <t>2016-09-05T18:25:21.249967</t>
   </si>
   <si>
     <t>2016-12-19T18:19:32.496552</t>
@@ -342,8 +397,7 @@
     <t>d9a963ea-8b1d-4ca3-9dd9-07a4773e8c23</t>
   </si>
   <si>
-    <t>http://datos.jus.gob.ar/dataset/base-de-datos-legislativos-infoleg
-</t>
+    <t>http://datos.jus.gob.ar/dataset/base-de-datos-legislativos-infoleg</t>
   </si>
   <si>
     <t>http://datos.jus.gob.ar/</t>
@@ -352,19 +406,16 @@
     <t>Open Data Commons Open Database License (ODbL)</t>
   </si>
   <si>
-    <t>Centros de Acceso a la Justicia -CAJ-
-</t>
+    <t>Centros de Acceso a la Justicia -CAJ-</t>
   </si>
   <si>
     <t>Este conjunto de datos contiene la información correspondiente a los Centros de Acceso a la Justicia -CAJ- que están activos. Los CAJ tienen por objetivo promover y facilitar el acceso a la justicia de los sectores más vulnerables, a través de asesoramiento y atención profesional, ya sea jurídico o psicosocial.</t>
   </si>
   <si>
-    <t>Ministerio de Justicia y Derechos Humanos. Subsecretaría de Acceso a la Justicia. Dirección Nacional de Acceso a la Justicia
-</t>
-  </si>
-  <si>
-    <t>rcoutenceau@jus.gov.ar
-</t>
+    <t>Ministerio de Justicia y Derechos Humanos. Subsecretaría de Acceso a la Justicia. Dirección Nacional de Acceso a la Justicia</t>
+  </si>
+  <si>
+    <t>rcoutenceau@jus.gov.ar</t>
   </si>
   <si>
     <t>CAJ,acceso a justicia,acceso a la justicia,asesoramiento jurídico,casas de justicia,justicia,vulnerable</t>
@@ -373,20 +424,16 @@
     <t>R/P3M</t>
   </si>
   <si>
-    <t>2016-09-08T15:01:56.463663
-</t>
-  </si>
-  <si>
-    <t>2016-11-30T14:19:05.433974
-</t>
-  </si>
-  <si>
-    <t>9775fcdf-99b9-47f6-87ae-6d46cfd15b40
-</t>
-  </si>
-  <si>
-    <t>http://datos.jus.gob.ar/dataset/centros-de-acceso-a-la-justicia
-</t>
+    <t>2016-09-08T15:01:56.463663</t>
+  </si>
+  <si>
+    <t>2016-11-30T14:19:05.433974</t>
+  </si>
+  <si>
+    <t>9775fcdf-99b9-47f6-87ae-6d46cfd15b40</t>
+  </si>
+  <si>
+    <t>http://datos.jus.gob.ar/dataset/centros-de-acceso-a-la-justicia</t>
   </si>
   <si>
     <t>Sistema de Consulta Nacional de Rebeldías y Capturas - Co.Na.R.C.</t>
@@ -395,51 +442,40 @@
     <t>La base Co.Na.R.C., creada a partir de la sanción del decreto 346/2009, se conforma con las comunicaciones que los tribunales realizan al Registro Nacional de Reincidencia de toda medida restrictiva a la libertad ambulatoria que se dicta en el marco de una causa penal, en cualquier jurisdicción del país (ámbito federal, nacional, provincial y de la CABA).  La base sólo refleja las órdenes de detención vigentes hasta las 7:00 hs. de la fecha de actualización.</t>
   </si>
   <si>
-    <t>Ministerio de Justicia. Subsecretaría de Asuntos Registrales. Direccion Nacional Registro Nacional de Reincidencia
-</t>
-  </si>
-  <si>
-    <t>fmichele@dnrec.jus.gov.ar
-</t>
-  </si>
-  <si>
-    <t>mpolimeni@dnrec.jus.gov.ar
-</t>
-  </si>
-  <si>
-    <t>
-capturas,detención,rebeldías</t>
+    <t>Ministerio de Justicia. Subsecretaría de Asuntos Registrales. Direccion Nacional Registro Nacional de Reincidencia</t>
+  </si>
+  <si>
+    <t>fmichele@dnrec.jus.gov.ar</t>
+  </si>
+  <si>
+    <t>mpolimeni@dnrec.jus.gov.ar</t>
+  </si>
+  <si>
+    <t>capturas,detención,rebeldías</t>
   </si>
   <si>
     <t>R/P1D</t>
   </si>
   <si>
-    <t>2016-09-28T14:57:47.665668
-</t>
-  </si>
-  <si>
-    <t>2016-12-21T12:08:10.905736
-</t>
-  </si>
-  <si>
-    <t>e042c362-ff39-476f-9328-056a9de753f0
-</t>
-  </si>
-  <si>
-    <t>http://datos.jus.gob.ar/dataset/conarc
-</t>
-  </si>
-  <si>
-    <t>Declaración Jurada Patrimonial Integral de carácter público
-</t>
-  </si>
-  <si>
-    <t>Datos correspondiente a las Declaraciones Juradas Patrimoniales Integrales presentadas por los sujetos obligados conforme lo normado en la Ley de Ética Pública 25.188 modificada por la Ley 26.857, reglamentada por el Decreto Nro. 895/2013 y la Resolución General AFIP Nro. 3511/2013 y Resolución M.J. y D.H. Nro. 1695/2013. La utilización de este conjunto de datos se encuentra regulada por el Art. 11 de la Ley de Ética Pública 25.188.
-</t>
-  </si>
-  <si>
-    <t>Ministerio de Justicia y Derechos Humanos. Oficina Anticorrupción.
-</t>
+    <t>2016-09-28T14:57:47.665668</t>
+  </si>
+  <si>
+    <t>2016-12-21T12:08:10.905736</t>
+  </si>
+  <si>
+    <t>e042c362-ff39-476f-9328-056a9de753f0</t>
+  </si>
+  <si>
+    <t>http://datos.jus.gob.ar/dataset/conarc</t>
+  </si>
+  <si>
+    <t>Declaración Jurada Patrimonial Integral de carácter público</t>
+  </si>
+  <si>
+    <t>Datos correspondiente a las Declaraciones Juradas Patrimoniales Integrales presentadas por los sujetos obligados conforme lo normado en la Ley de Ética Pública 25.188 modificada por la Ley 26.857, reglamentada por el Decreto Nro. 895/2013 y la Resolución General AFIP Nro. 3511/2013 y Resolución M.J. y D.H. Nro. 1695/2013. La utilización de este conjunto de datos se encuentra regulada por el Art. 11 de la Ley de Ética Pública 25.188.</t>
+  </si>
+  <si>
+    <t>Ministerio de Justicia y Derechos Humanos. Oficina Anticorrupción.</t>
   </si>
   <si>
     <t>distribution_accessURL</t>
@@ -448,8 +484,7 @@
     <t>uniddjjoa@jus.gov.ar</t>
   </si>
   <si>
-    <t>uniddjjoa@jus.gov.ar
-</t>
+    <t>uniddjjoa@jus.gov.ar</t>
   </si>
   <si>
     <t>DDJJ,Ley 25188,Ley 26857,anticorrupción,
@@ -459,20 +494,16 @@
     <t>eventual</t>
   </si>
   <si>
-    <t>2016-09-09T21:47:48.029246
-</t>
-  </si>
-  <si>
-    <t>2016-11-30T14:17:38.868492
-</t>
-  </si>
-  <si>
-    <t>4680199f-6234-4262-8a2a-8f7993bf784d
-</t>
-  </si>
-  <si>
-    <t>http://datos.jus.gob.ar/dataset/declaraciones-juradas-patrimoniales-integrales
-</t>
+    <t>2016-09-09T21:47:48.029246</t>
+  </si>
+  <si>
+    <t>2016-11-30T14:17:38.868492</t>
+  </si>
+  <si>
+    <t>4680199f-6234-4262-8a2a-8f7993bf784d</t>
+  </si>
+  <si>
+    <t>http://datos.jus.gob.ar/dataset/declaraciones-juradas-patrimoniales-integrales</t>
   </si>
   <si>
     <t>distribution_description</t>
@@ -529,8 +560,7 @@
     <t>da045e06-35cb-4bdd-9b5e-ddee6712c86c</t>
   </si>
   <si>
-    <t>http://datos.jus.gob.ar/dataset/entidades-constituidas-en-la-inspeccion-general-de-justicia-igj
-</t>
+    <t>http://datos.jus.gob.ar/dataset/entidades-constituidas-en-la-inspeccion-general-de-justicia-igj</t>
   </si>
   <si>
     <t>field_title</t>
@@ -566,8 +596,7 @@
     <t>de4560f4-8620-4cb5-a3a5-e3e5684c0e45</t>
   </si>
   <si>
-    <t>http://datos.jus.gob.ar/dataset/inscripciones-iniciales-de-automotores-y-motovehiculos
-</t>
+    <t>http://datos.jus.gob.ar/dataset/inscripciones-iniciales-de-automotores-y-motovehiculos</t>
   </si>
   <si>
     <t>field_type</t>
@@ -606,12 +635,10 @@
     <t>6d0e08b3-041c-40c1-9ea6-962db3747677</t>
   </si>
   <si>
-    <t>http://datos.jus.gob.ar/dataset/internos-del-servicio-penitenciario-federal-spf
-</t>
-  </si>
-  <si>
-    <t>http://datos.jus.gob.ar/dataset/d9a963ea-8b1d-4ca3-9dd9-07a4773e8c23/resource/8db246a2-48dd-4f2f-b08e-ab6293747882/download/baseinfolegnormativanacional.csv
-</t>
+    <t>http://datos.jus.gob.ar/dataset/internos-del-servicio-penitenciario-federal-spf</t>
+  </si>
+  <si>
+    <t>http://datos.jus.gob.ar/dataset/d9a963ea-8b1d-4ca3-9dd9-07a4773e8c23/resource/8db246a2-48dd-4f2f-b08e-ab6293747882/download/baseinfolegnormativanacional.csv</t>
   </si>
   <si>
     <t>Listado de Registros Seccionales de la Dirección Nacional de Registros Nacionales de la Propiedad Automotor y Créditos Prendarios</t>
@@ -623,15 +650,13 @@
     <t>2016-09-29T11:17:50.274309</t>
   </si>
   <si>
-    <t>2016-12-19T12:38:58.700747
-</t>
+    <t>2016-12-19T12:38:58.700747</t>
   </si>
   <si>
     <t>En este conjunto de datos se detallan los datos de los Registros Seccionales donde se realizan los trámites registrales de los vehículos (automotores, motovehículos y maquinarias agrícolas, viales e industriales y créditos prendarios) de todo el país.</t>
   </si>
   <si>
-    <t>d9a963ea-8b1d-4ca3-9dd9-07a4773e8c23
-</t>
+    <t>d9a963ea-8b1d-4ca3-9dd9-07a4773e8c23</t>
   </si>
   <si>
     <t>id_norma</t>
@@ -670,8 +695,7 @@
     <t>Número de norma.</t>
   </si>
   <si>
-    <t>http://datos.jus.gob.ar/dataset/d9a963ea-8b1d-4ca3-9dd9-07a4773e8c23/resource/d9fbf1d5-679e-4833-bcdc-3a8f58523d18/download/basecomplementariainfolegnormasmodificadas.csv
-</t>
+    <t>http://datos.jus.gob.ar/dataset/d9a963ea-8b1d-4ca3-9dd9-07a4773e8c23/resource/d9fbf1d5-679e-4833-bcdc-3a8f58523d18/download/basecomplementariainfolegnormasmodificadas.csv</t>
   </si>
   <si>
     <t>2016-12-01T20:11:25.275826</t>
@@ -686,15 +710,13 @@
     <t>indica la clase de la norma.</t>
   </si>
   <si>
-    <t>http://datos.jus.gob.ar/dataset/listado-de-registros-seccionales-de-la-dnrnpa
-</t>
+    <t>http://datos.jus.gob.ar/dataset/listado-de-registros-seccionales-de-la-dnrnpa</t>
   </si>
   <si>
     <t>organismo_origen</t>
   </si>
   <si>
-    <t>Base Complementaria Infoleg de Normas Modificadas
-</t>
+    <t>Base Complementaria Infoleg de Normas Modificadas</t>
   </si>
   <si>
     <t>2016-10-14T16:02:49.841535</t>
@@ -703,8 +725,7 @@
     <t>Organismo de origen. Organismo que dictó/ sancionó la norma.</t>
   </si>
   <si>
-    <t>2016-12-19T14:48:05.348064
-</t>
+    <t>2016-12-19T14:48:05.348064</t>
   </si>
   <si>
     <t>numero_boletin</t>
@@ -713,8 +734,7 @@
     <t>Número de boletin oficial en el que se publicó la norma.</t>
   </si>
   <si>
-    <t>http://datos.jus.gob.ar/dataset/base-de-datos-legislativos-infoleg/archivo/f9170086-6538-44f1-8c7e-3e193c1fea7f
-</t>
+    <t>http://datos.jus.gob.ar/dataset/base-de-datos-legislativos-infoleg/archivo/f9170086-6538-44f1-8c7e-3e193c1fea7f</t>
   </si>
   <si>
     <t>fecha_boletin</t>
@@ -744,8 +764,7 @@
     <t>fecha_sancion</t>
   </si>
   <si>
-    <t>http://datos.jus.gob.ar/dataset/d9a963ea-8b1d-4ca3-9dd9-07a4773e8c23/resource/f9170086-6538-44f1-8c7e-3e193c1fea7f/download/basecomplementariainfolegnormasmodificatorias.csv
-</t>
+    <t>http://datos.jus.gob.ar/dataset/d9a963ea-8b1d-4ca3-9dd9-07a4773e8c23/resource/f9170086-6538-44f1-8c7e-3e193c1fea7f/download/basecomplementariainfolegnormasmodificatorias.csv</t>
   </si>
   <si>
     <t>Fecha en la que la norma se sancionó/dictó  (formato: DD/MM/AAAA).</t>
@@ -760,8 +779,7 @@
     <t>cargo,concurso,defensor,federal,fiscal,juez,justicia,magistrado,nacional,subrogante,vacante,órgano</t>
   </si>
   <si>
-    <t>Base Complementaria Infoleg de Normas Modificatorias
-</t>
+    <t>Base Complementaria Infoleg de Normas Modificatorias</t>
   </si>
   <si>
     <t>titulo_resumido</t>
@@ -773,8 +791,7 @@
     <t>Breve resumen del título.</t>
   </si>
   <si>
-    <t>2016-10-18T17:26:58.415087
-</t>
+    <t>2016-10-18T17:26:58.415087</t>
   </si>
   <si>
     <t>2016-12-07T20:43:07.256061</t>
@@ -783,15 +800,13 @@
     <t>3c18d46e-729e-4973-8efd-f54cab18b7e3</t>
   </si>
   <si>
-    <t>2016-12-19T14:47:21.330355
-</t>
+    <t>2016-12-19T14:47:21.330355</t>
   </si>
   <si>
     <t>titulo_sumario</t>
   </si>
   <si>
-    <t>http://datos.jus.gob.ar/dataset/magistrados-justicia-federal-y-de-la-justicia-nacional
-</t>
+    <t>http://datos.jus.gob.ar/dataset/magistrados-justicia-federal-y-de-la-justicia-nacional</t>
   </si>
   <si>
     <t>Sumario del título en una o dos palabras. (Ej: "sistema integrado de jubilaciones")</t>
@@ -842,15 +857,13 @@
     <t>Hipervínculo al texto actualizado de la norma.</t>
   </si>
   <si>
-    <t>Centros de Acceso a la Justicia activos
-</t>
+    <t>Centros de Acceso a la Justicia activos</t>
   </si>
   <si>
     <t>2016-12-05T20:09:47.885628</t>
   </si>
   <si>
-    <t>CSV
-</t>
+    <t>CSV</t>
   </si>
   <si>
     <t>a9767469-d903-4158-aa76-b21dd37e8aff</t>
@@ -859,15 +872,13 @@
     <t>modificada_por</t>
   </si>
   <si>
-    <t>http://datos.jus.gob.ar/dataset/mediaciones-prejudiciales-y-judiciales
-</t>
+    <t>http://datos.jus.gob.ar/dataset/mediaciones-prejudiciales-y-judiciales</t>
   </si>
   <si>
     <t>Identificar único de la norma que la modifica.</t>
   </si>
   <si>
-    <t>http://datos.jus.gob.ar/dataset/9775fcdf-99b9-47f6-87ae-6d46cfd15b40/resource/906a1daf-cb0c-4765-98d4-40b0f8caf48b/download/centros-acceso-justicia-activos.csv
-</t>
+    <t>http://datos.jus.gob.ar/dataset/9775fcdf-99b9-47f6-87ae-6d46cfd15b40/resource/906a1daf-cb0c-4765-98d4-40b0f8caf48b/download/centros-acceso-justicia-activos.csv</t>
   </si>
   <si>
     <t>modifica_a</t>
@@ -882,15 +893,13 @@
     <t>Centros de Acceso a la Justicia (CAJ)</t>
   </si>
   <si>
-    <t>2016-10-06T14:03:39.969278
-</t>
+    <t>2016-10-06T14:03:39.969278</t>
   </si>
   <si>
     <t>Se registran los femicidios y homicidios agravados por el género desde el año 2012 a la fecha. La base se nutre de diversas fuentes: articulos de prensa escrita, denuncias policiales y judiciales, denuncias realizadas ante la Secretaría de Derechos Humanos.</t>
   </si>
   <si>
-    <t>2016-11-14T16:24:13.596458
-</t>
+    <t>2016-11-14T16:24:13.596458</t>
   </si>
   <si>
     <t>id_norma_modificada</t>
@@ -914,19 +923,16 @@
     <t>Identificador único de la norma modificatoria dentro de la base de datos.</t>
   </si>
   <si>
-    <t>Sistema de Consulta Nacional de Rebeldías y Capturas (base Co.Na.R.C.) vigentes al 21-12-2016
-</t>
-  </si>
-  <si>
-    <t>
-femicidios,genero,homicidios,violencia</t>
+    <t>Sistema de Consulta Nacional de Rebeldías y Capturas (base Co.Na.R.C.) vigentes al 21-12-2016</t>
+  </si>
+  <si>
+    <t>femicidios,genero,homicidios,violencia</t>
   </si>
   <si>
     <t>2016-09-14T14:04:25.296524</t>
   </si>
   <si>
-    <t>http://datos.jus.gob.ar/dataset/e042c362-ff39-476f-9328-056a9de753f0/resource/a95d0e79-08c4-49b9-88b8-d569484bf1d7/download/rebeldias-y-capturas.csv
-</t>
+    <t>http://datos.jus.gob.ar/dataset/e042c362-ff39-476f-9328-056a9de753f0/resource/a95d0e79-08c4-49b9-88b8-d569484bf1d7/download/rebeldias-y-capturas.csv</t>
   </si>
   <si>
     <t>2016-12-05T17:13:03.888139</t>
@@ -935,19 +941,16 @@
     <t>27bb9b2c-521b-406c-bdf9-98110ef73f34</t>
   </si>
   <si>
-    <t>http://datos.jus.gob.ar/dataset/registro-sistematizacion-y-seguimiento-de-femicidios-y-homicidios-agravados-por-el-genero
-</t>
-  </si>
-  <si>
-    <t>Sistema de Consulta Nacional de Rebeldías y Capturas
-</t>
+    <t>http://datos.jus.gob.ar/dataset/registro-sistematizacion-y-seguimiento-de-femicidios-y-homicidios-agravados-por-el-genero</t>
+  </si>
+  <si>
+    <t>Sistema de Consulta Nacional de Rebeldías y Capturas</t>
   </si>
   <si>
     <t>2016-10-06T13:36:46.495627</t>
   </si>
   <si>
-    <t>2016-12-21T09:04:05.877238
-</t>
+    <t>2016-12-21T09:04:05.877238</t>
   </si>
   <si>
     <t>Indica la clase de la norma.</t>
@@ -959,26 +962,22 @@
     <t>Registro Unificado de Víctimas del Terrorismo de Estado -RUVTE-</t>
   </si>
   <si>
-    <t>Declaraciones Juradas Patrimoniales Integrales para el año fiscal 2015
-</t>
+    <t>Declaraciones Juradas Patrimoniales Integrales para el año fiscal 2015</t>
   </si>
   <si>
     <t>Fecha en la que la norma se publicó en el boletín oficial  (formato: DD/MM/AAAA).</t>
   </si>
   <si>
-    <t>http://datos.jus.gob.ar/dataset/4680199f-6234-4262-8a2a-8f7993bf784d/resource/b029969c-85a7-4adb-afe1-33165e835517/download/declaraciones-juradas-2015.csv
-</t>
+    <t>http://datos.jus.gob.ar/dataset/4680199f-6234-4262-8a2a-8f7993bf784d/resource/b029969c-85a7-4adb-afe1-33165e835517/download/declaraciones-juradas-2015.csv</t>
   </si>
   <si>
     <t>Registro unificado del listado de Víctimas del accionar represivo ilegal del Estado argentino entre 1966 y 1983 (víctimas de desaparición forzada y de asesinato) y del listado de casos en investigación incluidos en el listado de la Conadep, sin denuncia formal ante la Secretaría de Derechos Humanos y Pluralismo Cultural de la Nación, que revisten la categoría de “presunción de desaparición forzada”.</t>
   </si>
   <si>
-    <t>2016-09-09T18:53:26.160150
-</t>
-  </si>
-  <si>
-    <t>2016-09-29T16:52:23.970945
-</t>
+    <t>2016-09-09T18:53:26.160150</t>
+  </si>
+  <si>
+    <t>2016-09-29T16:52:23.970945</t>
   </si>
   <si>
     <t>Ministerio de Justicia y Derechos Humanos. Secretaría de Derechos Humanos y Pluralismo Cultural. Registro Unificado de Víctimas del Terrorismo de Estado</t>
@@ -990,16 +989,13 @@
     <t>http://datos.jus.gob.ar/dataset/declaraciones-juradas-patrimoniales-integrales/archivo/0bd85cd7-ef0a-4e62-be7b-6d58db17ebbc</t>
   </si>
   <si>
-    <t>Declaraciones Juradas Patrimoniales Integrales para el año fiscal 2014
-</t>
-  </si>
-  <si>
-    <t>
-desaparecidos,desaparición forzada,represión,víctimas</t>
-  </si>
-  <si>
-    <t>http://datos.jus.gob.ar/dataset/4680199f-6234-4262-8a2a-8f7993bf784d/resource/0bd85cd7-ef0a-4e62-be7b-6d58db17ebbc/download/declaraciones-juradas-2014.csv
-</t>
+    <t>Declaraciones Juradas Patrimoniales Integrales para el año fiscal 2014</t>
+  </si>
+  <si>
+    <t>desaparecidos,desaparición forzada,represión,víctimas</t>
+  </si>
+  <si>
+    <t>http://datos.jus.gob.ar/dataset/4680199f-6234-4262-8a2a-8f7993bf784d/resource/0bd85cd7-ef0a-4e62-be7b-6d58db17ebbc/download/declaraciones-juradas-2014.csv</t>
   </si>
   <si>
     <t>2016-09-30T18:34:43.987076</t>
@@ -1011,30 +1007,25 @@
     <t>d43fa140-f43f-4cc2-8491-b1d8bb899de4</t>
   </si>
   <si>
-    <t>2016-09-28T16:16:22.346673
-</t>
-  </si>
-  <si>
-    <t>http://datos.jus.gob.ar/dataset/registro-unificado-de-victimas-del-terrorismo-de-estado-ruvte
-</t>
-  </si>
-  <si>
-    <t>2016-09-29T16:53:24.126454
-</t>
+    <t>2016-09-28T16:16:22.346673</t>
+  </si>
+  <si>
+    <t>http://datos.jus.gob.ar/dataset/registro-unificado-de-victimas-del-terrorismo-de-estado-ruvte</t>
+  </si>
+  <si>
+    <t>2016-09-29T16:53:24.126454</t>
   </si>
   <si>
     <t>http://datos.jus.gob.ar/dataset/declaraciones-juradas-patrimoniales-integrales/archivo/357e0886-2b15-481b-9e4b-d7f663c214bb</t>
   </si>
   <si>
-    <t>Declaraciones Juradas Patrimoniales Integrales para el año fiscal 2013
-</t>
+    <t>Declaraciones Juradas Patrimoniales Integrales para el año fiscal 2013</t>
   </si>
   <si>
     <t>Sistema Nacional de Estadísticas sobre Ejecución de la Pena – SNEEP</t>
   </si>
   <si>
-    <t>http://datos.jus.gob.ar/dataset/4680199f-6234-4262-8a2a-8f7993bf784d/resource/357e0886-2b15-481b-9e4b-d7f663c214bb/download/declaraciones-juradas-2013.csv
-</t>
+    <t>http://datos.jus.gob.ar/dataset/4680199f-6234-4262-8a2a-8f7993bf784d/resource/357e0886-2b15-481b-9e4b-d7f663c214bb/download/declaraciones-juradas-2013.csv</t>
   </si>
   <si>
     <t>En este cuerpo de datos se detalla los datos recopilados en el censo realizado sobre el total de la población detenida al día 31 de diciembre de cada año, en cada establecimiento de la República Argentina. La unidad de análisis son las personas alojadas en dichos establecimientos.</t>
@@ -1046,12 +1037,10 @@
     <t>CGonzalezGuerra@jus.gov.ar</t>
   </si>
   <si>
-    <t>2016-09-28T16:17:05.354649
-</t>
-  </si>
-  <si>
-    <t>2016-09-29T16:53:46.438911
-</t>
+    <t>2016-09-28T16:17:05.354649</t>
+  </si>
+  <si>
+    <t>2016-09-29T16:53:46.438911</t>
   </si>
   <si>
     <t>4680199f-6234-4262-8a2a-8f7993bf784d</t>
@@ -1060,8 +1049,7 @@
     <t>politica-criminal,sistema-penitenciario</t>
   </si>
   <si>
-    <t>
-SNEEP,SPF,cárceles,ejecución de la pena,establecimientos penitenciarios,personas privadas de la libertad,presos,prisión</t>
+    <t>SNEEP,SPF,cárceles,ejecución de la pena,establecimientos penitenciarios,personas privadas de la libertad,presos,prisión</t>
   </si>
   <si>
     <t>R/P1Y</t>
@@ -1082,8 +1070,7 @@
     <t>Indica el nombre de la oficina identificada por lugar.</t>
   </si>
   <si>
-    <t>http://datos.jus.gob.ar/dataset/sneep
-</t>
+    <t>http://datos.jus.gob.ar/dataset/sneep</t>
   </si>
   <si>
     <t>fecha_apertura</t>
@@ -1108,8 +1095,7 @@
  Los datos son actualizados en forma diaria y son vistos hasta las 00:00 horas del día siguiente del vencimiento de la publicación. Resolución ANMaC N°0009/2016.</t>
   </si>
   <si>
-    <t>http://datos.jus.gob.ar/dataset/declaraciones-juradas-patrimoniales-integrales/archivo/daad6625-2610-4d7e-b4fc-45a235e48f07
-</t>
+    <t>http://datos.jus.gob.ar/dataset/declaraciones-juradas-patrimoniales-integrales/archivo/daad6625-2610-4d7e-b4fc-45a235e48f07</t>
   </si>
   <si>
     <t>Localidad en la que se ubica el centro.</t>
@@ -1157,8 +1143,7 @@
     <t>0a0c3def-3d81-4850-854c-7af25831250b</t>
   </si>
   <si>
-    <t>http://datos.jus.gob.ar/dataset/solicitudes-condicion-legitimo-usuario-armas-fuego
-</t>
+    <t>http://datos.jus.gob.ar/dataset/solicitudes-condicion-legitimo-usuario-armas-fuego</t>
   </si>
   <si>
     <t>responsable</t>
@@ -1204,15 +1189,13 @@
     <t>2016-12-16T14:50:45.413434</t>
   </si>
   <si>
-    <t>http://datos.jus.gob.ar/dataset/entidades-constituidas-en-la-inspeccion-general-de-justicia-igj/archivo/c81a673f-50e4-4d3e-8ff5-8e623adf8161
-</t>
+    <t>http://datos.jus.gob.ar/dataset/entidades-constituidas-en-la-inspeccion-general-de-justicia-igj/archivo/c81a673f-50e4-4d3e-8ff5-8e623adf8161</t>
   </si>
   <si>
     <t>35278d98-c274-4612-9d1d-72d0d0923368</t>
   </si>
   <si>
-    <t>http://datos.jus.gob.ar/dataset/solicitudes-de-autorizacion-de-portacion-de-armas-de-fuego
-</t>
+    <t>http://datos.jus.gob.ar/dataset/solicitudes-de-autorizacion-de-portacion-de-armas-de-fuego</t>
   </si>
   <si>
     <t>apellidos</t>
@@ -1263,12 +1246,10 @@
     <t>fecha_nacimiento</t>
   </si>
   <si>
-    <t>http://datos.jus.gob.ar/dataset/entidades-constituidas-en-la-inspeccion-general-de-justicia-igj/archivo/ed11b717-d6d1-411d-b040-bfc0987cd72c
-</t>
-  </si>
-  <si>
-    <t>
-denuncias,derechos humanos,violación a los derechos humanos,violencia institucional</t>
+    <t>http://datos.jus.gob.ar/dataset/entidades-constituidas-en-la-inspeccion-general-de-justicia-igj/archivo/ed11b717-d6d1-411d-b040-bfc0987cd72c</t>
+  </si>
+  <si>
+    <t>denuncias,derechos humanos,violación a los derechos humanos,violencia institucional</t>
   </si>
   <si>
     <t>Domicilios de entidades constituidas en la IGJ</t>
@@ -1289,8 +1270,7 @@
     <t>Fecha de nacimiento en formato DD/MM/AAAA.</t>
   </si>
   <si>
-    <t>http://datos.jus.gob.ar/dataset/unidad-de-registro-sistematizacion-y-seguimiento-de-hechos-de-violencia-institucional
-</t>
+    <t>http://datos.jus.gob.ar/dataset/unidad-de-registro-sistematizacion-y-seguimiento-de-hechos-de-violencia-institucional</t>
   </si>
   <si>
     <t>nacionalidad</t>
@@ -1320,8 +1300,7 @@
     <t>Tipo de delito.</t>
   </si>
   <si>
-    <t>http://datos.jus.gob.ar/dataset/entidades-constituidas-en-la-inspeccion-general-de-justicia-igj/archivo/079c1104-aae4-4fe1-9474-e44e99054c9d
-</t>
+    <t>http://datos.jus.gob.ar/dataset/entidades-constituidas-en-la-inspeccion-general-de-justicia-igj/archivo/079c1104-aae4-4fe1-9474-e44e99054c9d</t>
   </si>
   <si>
     <t>organismo</t>
@@ -1357,8 +1336,7 @@
     <t>2016-10-20T10:48:32.582651</t>
   </si>
   <si>
-    <t>http://datos.jus.gob.ar/dataset/entidades-constituidas-en-la-inspeccion-general-de-justicia-igj/archivo/ad6835d8-0d6b-42dc-bb8f-2641af5ddf01
-</t>
+    <t>http://datos.jus.gob.ar/dataset/entidades-constituidas-en-la-inspeccion-general-de-justicia-igj/archivo/ad6835d8-0d6b-42dc-bb8f-2641af5ddf01</t>
   </si>
   <si>
     <t>Balances presentados por entidades constituidas en la IGJ</t>
@@ -1376,8 +1354,7 @@
     <t>2016-10-20T13:17:57.625351</t>
   </si>
   <si>
-    <t>http://datos.jus.gob.ar/dataset/entidades-constituidas-en-la-inspeccion-general-de-justicia-igj/archivo/75ec7f99-7088-4367-9ca4-d014d65f4a0a
-</t>
+    <t>http://datos.jus.gob.ar/dataset/entidades-constituidas-en-la-inspeccion-general-de-justicia-igj/archivo/75ec7f99-7088-4367-9ca4-d014d65f4a0a</t>
   </si>
   <si>
     <t>Asambleas de entidades constituidas en la IGJ</t>
@@ -1395,8 +1372,7 @@
     <t>2016-10-19T17:47:07.824579</t>
   </si>
   <si>
-    <t>http://datos.jus.gob.ar/dataset/entidades-constituidas-en-la-inspeccion-general-de-justicia-igj/archivo/69ba7f4a-b2d4-476e-9feb-9616fee79677
-</t>
+    <t>http://datos.jus.gob.ar/dataset/entidades-constituidas-en-la-inspeccion-general-de-justicia-igj/archivo/69ba7f4a-b2d4-476e-9feb-9616fee79677</t>
   </si>
   <si>
     <t>Autoridades de entidades constituidas en la IGJ.</t>
@@ -1414,8 +1390,7 @@
     <t>2016-11-18T12:50:15.336412</t>
   </si>
   <si>
-    <t>http://datos.jus.gob.ar/dataset/entidades-constituidas-en-la-inspeccion-general-de-justicia-igj/archivo/055e1b3a-c127-436c-829b-7e2cc9a4d9c8
-</t>
+    <t>http://datos.jus.gob.ar/dataset/entidades-constituidas-en-la-inspeccion-general-de-justicia-igj/archivo/055e1b3a-c127-436c-829b-7e2cc9a4d9c8</t>
   </si>
   <si>
     <t>http://datos.jus.gob.ar/dataset/da045e06-35cb-4bdd-9b5e-ddee6712c86c/resource/055e1b3a-c127-436c-829b-7e2cc9a4d9c8/download/igj-entidades.csv</t>
@@ -1430,8 +1405,7 @@
     <t>2016-11-17T14:51:22.001319</t>
   </si>
   <si>
-    <t>http://datos.jus.gob.ar/dataset/entidades-constituidas-en-la-inspeccion-general-de-justicia-igj/archivo/2a8472e3-3ec6-4e6e-8baf-d53963f22643
-</t>
+    <t>http://datos.jus.gob.ar/dataset/entidades-constituidas-en-la-inspeccion-general-de-justicia-igj/archivo/2a8472e3-3ec6-4e6e-8baf-d53963f22643</t>
   </si>
   <si>
     <t>http://datos.jus.gob.ar/dataset/da045e06-35cb-4bdd-9b5e-ddee6712c86c/resource/2a8472e3-3ec6-4e6e-8baf-d53963f22643/download/igj-balances.csv</t>
@@ -1470,8 +1444,7 @@
     <t>Themes extraidos de: "http://datos.jus.gob.ar/api/3/action/help_show?name=group_list"</t>
   </si>
   <si>
-    <t>http://datos.jus.gob.ar/dataset/entidades-constituidas-en-la-inspeccion-general-de-justicia-igj/archivo/52e983b1-e633-4e1d-94b9-3be23c0a3a8f
-</t>
+    <t>http://datos.jus.gob.ar/dataset/entidades-constituidas-en-la-inspeccion-general-de-justicia-igj/archivo/52e983b1-e633-4e1d-94b9-3be23c0a3a8f</t>
   </si>
   <si>
     <t>http://datos.jus.gob.ar/dataset/da045e06-35cb-4bdd-9b5e-ddee6712c86c/resource/52e983b1-e633-4e1d-94b9-3be23c0a3a8f/download/igj-asambleas.csv</t>
@@ -1486,8 +1459,7 @@
     <t>2016-11-17T15:16:07.094117</t>
   </si>
   <si>
-    <t>http://datos.jus.gob.ar/dataset/entidades-constituidas-en-la-inspeccion-general-de-justicia-igj/archivo/c0fdac96-66ba-4c28-9a54-d4f7f27fd5f3
-</t>
+    <t>http://datos.jus.gob.ar/dataset/entidades-constituidas-en-la-inspeccion-general-de-justicia-igj/archivo/c0fdac96-66ba-4c28-9a54-d4f7f27fd5f3</t>
   </si>
   <si>
     <t>http://datos.jus.gob.ar/dataset/da045e06-35cb-4bdd-9b5e-ddee6712c86c/resource/c0fdac96-66ba-4c28-9a54-d4f7f27fd5f3/download/igj-domicilios.csv</t>
@@ -1502,8 +1474,7 @@
     <t>2016-11-17T15:16:46.319333</t>
   </si>
   <si>
-    <t>http://datos.jus.gob.ar/dataset/entidades-constituidas-en-la-inspeccion-general-de-justicia-igj/archivo/b2df002f-c621-46e6-bb4f-e90be984f1f5
-</t>
+    <t>http://datos.jus.gob.ar/dataset/entidades-constituidas-en-la-inspeccion-general-de-justicia-igj/archivo/b2df002f-c621-46e6-bb4f-e90be984f1f5</t>
   </si>
   <si>
     <t>http://datos.jus.gob.ar/dataset/da045e06-35cb-4bdd-9b5e-ddee6712c86c/resource/b2df002f-c621-46e6-bb4f-e90be984f1f5/download/igj-entidades.csv</t>
@@ -1518,8 +1489,7 @@
     <t>2016-12-07T09:49:39.478384</t>
   </si>
   <si>
-    <t>http://datos.jus.gob.ar/dataset/entidades-constituidas-en-la-inspeccion-general-de-justicia-igj/archivo/b955c68f-cc82-4e72-9b08-d348ef59529a
-</t>
+    <t>http://datos.jus.gob.ar/dataset/entidades-constituidas-en-la-inspeccion-general-de-justicia-igj/archivo/b955c68f-cc82-4e72-9b08-d348ef59529a</t>
   </si>
   <si>
     <t>http://datos.jus.gob.ar/dataset/da045e06-35cb-4bdd-9b5e-ddee6712c86c/resource/b955c68f-cc82-4e72-9b08-d348ef59529a/download/igj-asambleas.csv</t>
@@ -1534,8 +1504,7 @@
     <t>2016-12-06T14:22:09.287806</t>
   </si>
   <si>
-    <t>http://datos.jus.gob.ar/dataset/entidades-constituidas-en-la-inspeccion-general-de-justicia-igj/archivo/fafa4336-1e8e-411c-bb42-4f90300002e6
-</t>
+    <t>http://datos.jus.gob.ar/dataset/entidades-constituidas-en-la-inspeccion-general-de-justicia-igj/archivo/fafa4336-1e8e-411c-bb42-4f90300002e6</t>
   </si>
   <si>
     <t>http://datos.jus.gob.ar/dataset/da045e06-35cb-4bdd-9b5e-ddee6712c86c/resource/fafa4336-1e8e-411c-bb42-4f90300002e6/download/igj-autoridades.csv</t>
@@ -1550,8 +1519,7 @@
     <t>2016-12-07T09:58:03.676396</t>
   </si>
   <si>
-    <t>http://datos.jus.gob.ar/dataset/entidades-constituidas-en-la-inspeccion-general-de-justicia-igj/archivo/dc7d85b2-a695-4a9d-91e8-65de43b00b30
-</t>
+    <t>http://datos.jus.gob.ar/dataset/entidades-constituidas-en-la-inspeccion-general-de-justicia-igj/archivo/dc7d85b2-a695-4a9d-91e8-65de43b00b30</t>
   </si>
   <si>
     <t>http://datos.jus.gob.ar/dataset/da045e06-35cb-4bdd-9b5e-ddee6712c86c/resource/dc7d85b2-a695-4a9d-91e8-65de43b00b30/download/igj-balances.csv</t>
@@ -1566,12 +1534,10 @@
     <t>2016-12-06T14:36:01.022532</t>
   </si>
   <si>
-    <t>Entidades constituidas en la Inspección General de Justicia
-</t>
-  </si>
-  <si>
-    <t>http://datos.jus.gob.ar/dataset/entidades-constituidas-en-la-inspeccion-general-de-justicia-igj/archivo/b7311dd0-0a40-4bcf-aead-dbc2250cef5a
-</t>
+    <t>Entidades constituidas en la Inspección General de Justicia</t>
+  </si>
+  <si>
+    <t>http://datos.jus.gob.ar/dataset/entidades-constituidas-en-la-inspeccion-general-de-justicia-igj/archivo/b7311dd0-0a40-4bcf-aead-dbc2250cef5a</t>
   </si>
   <si>
     <t>http://datos.jus.gob.ar/dataset/da045e06-35cb-4bdd-9b5e-ddee6712c86c/resource/b7311dd0-0a40-4bcf-aead-dbc2250cef5a/download/igj-domicilios.csv</t>
@@ -1586,8 +1552,7 @@
     <t>2016-12-06T11:15:38.575884</t>
   </si>
   <si>
-    <t>http://datos.jus.gob.ar/dataset/inscripciones-iniciales-de-automotores-y-motovehiculos/archivo/2436ab65-44da-4f45-a59d-5e09136e1df2
-</t>
+    <t>http://datos.jus.gob.ar/dataset/inscripciones-iniciales-de-automotores-y-motovehiculos/archivo/2436ab65-44da-4f45-a59d-5e09136e1df2</t>
   </si>
   <si>
     <t>Estadística mensual de inscripciones iniciales de automotores y motovehículos</t>
@@ -1605,8 +1570,7 @@
     <t>2016-12-05T15:00:51.294963</t>
   </si>
   <si>
-    <t>http://datos.jus.gob.ar/dataset/internos-del-servicio-penitenciario-federal-spf/archivo/47e53feb-ca88-4322-a663-e511485213a0
-</t>
+    <t>http://datos.jus.gob.ar/dataset/internos-del-servicio-penitenciario-federal-spf/archivo/47e53feb-ca88-4322-a663-e511485213a0</t>
   </si>
   <si>
     <t>Este conjunto de datos registra los condenados alojados en los establecimientos del Servicio Penitenciario Federal de todo el país.</t>
@@ -1624,8 +1588,7 @@
     <t>2016-11-18T11:17:16.127349</t>
   </si>
   <si>
-    <t>http://datos.jus.gob.ar/dataset/internos-del-servicio-penitenciario-federal-spf/archivo/ecc3d11d-ea79-43e6-81dd-fe6557cdbc08
-</t>
+    <t>http://datos.jus.gob.ar/dataset/internos-del-servicio-penitenciario-federal-spf/archivo/ecc3d11d-ea79-43e6-81dd-fe6557cdbc08</t>
   </si>
   <si>
     <t>Este conjunto de datos registra los inimputables alojados en los establecimientos del Servicio Penitenciario Federal de todo el país.</t>
@@ -1643,8 +1606,7 @@
     <t>2016-11-18T11:18:23.802030</t>
   </si>
   <si>
-    <t>http://datos.jus.gob.ar/dataset/internos-del-servicio-penitenciario-federal-spf/archivo/43b72420-1934-45d8-bcf1-c030f442dd85
-</t>
+    <t>http://datos.jus.gob.ar/dataset/internos-del-servicio-penitenciario-federal-spf/archivo/43b72420-1934-45d8-bcf1-c030f442dd85</t>
   </si>
   <si>
     <t>Este conjunto de datos registra los procesados alojados en los establecimientos del Servicio Penitenciario Federal de todo el país.</t>
@@ -1662,8 +1624,7 @@
     <t>2016-11-18T12:39:17.671667</t>
   </si>
   <si>
-    <t>http://datos.jus.gob.ar/dataset/internos-del-servicio-penitenciario-federal-spf/archivo/9e29e518-90d2-4338-9994-fe6eae9a6c9f
-</t>
+    <t>http://datos.jus.gob.ar/dataset/internos-del-servicio-penitenciario-federal-spf/archivo/9e29e518-90d2-4338-9994-fe6eae9a6c9f</t>
   </si>
   <si>
     <t>http://datos.jus.gob.ar/dataset/6d0e08b3-041c-40c1-9ea6-962db3747677/resource/9e29e518-90d2-4338-9994-fe6eae9a6c9f/download/internos-spf-inimputables-2016-10.csv</t>
@@ -1678,8 +1639,7 @@
     <t>2016-12-13T16:38:46.623707</t>
   </si>
   <si>
-    <t>http://datos.jus.gob.ar/dataset/internos-del-servicio-penitenciario-federal-spf/archivo/aea37ed5-9cbb-408f-a95e-86de7130b958
-</t>
+    <t>http://datos.jus.gob.ar/dataset/internos-del-servicio-penitenciario-federal-spf/archivo/aea37ed5-9cbb-408f-a95e-86de7130b958</t>
   </si>
   <si>
     <t>http://datos.jus.gob.ar/dataset/6d0e08b3-041c-40c1-9ea6-962db3747677/resource/aea37ed5-9cbb-408f-a95e-86de7130b958/download/internos-spf-condenados-2016-10.csv</t>
@@ -1694,8 +1654,7 @@
     <t>2016-12-06T11:51:15.724249</t>
   </si>
   <si>
-    <t>http://datos.jus.gob.ar/dataset/internos-del-servicio-penitenciario-federal-spf/archivo/28dd97a3-df32-442d-8f4e-2e845ce18c43
-</t>
+    <t>http://datos.jus.gob.ar/dataset/internos-del-servicio-penitenciario-federal-spf/archivo/28dd97a3-df32-442d-8f4e-2e845ce18c43</t>
   </si>
   <si>
     <t>http://datos.jus.gob.ar/dataset/6d0e08b3-041c-40c1-9ea6-962db3747677/resource/28dd97a3-df32-442d-8f4e-2e845ce18c43/download/internos-spf-procesados-2016-10.csv</t>
@@ -1710,8 +1669,7 @@
     <t>2016-12-12T17:15:11.324717</t>
   </si>
   <si>
-    <t>http://datos.jus.gob.ar/dataset/listado-de-registros-seccionales-de-la-dnrnpa/archivo/54bd9fa1-a059-4411-b146-457791e882f8
-</t>
+    <t>http://datos.jus.gob.ar/dataset/listado-de-registros-seccionales-de-la-dnrnpa/archivo/54bd9fa1-a059-4411-b146-457791e882f8</t>
   </si>
   <si>
     <t>Listado de Registros Seccionales de todo el país con competencia en automotores, motovehículos, maquinaria agrícola, vial e industrial y créditos prendarios.</t>
@@ -1729,8 +1687,7 @@
     <t>2016-12-01T17:11:05.351900</t>
   </si>
   <si>
-    <t>http://datos.jus.gob.ar/dataset/magistrados-justicia-federal-y-de-la-justicia-nacional/archivo/3c8c1fea-c97b-4368-b31b-da244d66adb3
-</t>
+    <t>http://datos.jus.gob.ar/dataset/magistrados-justicia-federal-y-de-la-justicia-nacional/archivo/3c8c1fea-c97b-4368-b31b-da244d66adb3</t>
   </si>
   <si>
     <t>Listado actual de jueces, fiscales y defensores de la Justicia Federal y de la Justicia Nacional. No se incluyen los magistrados de la Corte Suprema de Justicia de la Nación, de la Procuración General de la Nación ni de la Defensoría General de la Nación.</t>
@@ -1745,8 +1702,7 @@
     <t>2016-12-07T17:38:50.689433</t>
   </si>
   <si>
-    <t>http://datos.jus.gob.ar/dataset/magistrados-justicia-federal-y-de-la-justicia-nacional/archivo/ac34ee63-7e86-4f15-b57b-c6a35f71ea6e
-</t>
+    <t>http://datos.jus.gob.ar/dataset/magistrados-justicia-federal-y-de-la-justicia-nacional/archivo/ac34ee63-7e86-4f15-b57b-c6a35f71ea6e</t>
   </si>
   <si>
     <t>Designacion de jueces, fiscales y defensores de la Justicia Federal y de la Justicia Nacional</t>
@@ -1764,8 +1720,7 @@
     <t>2016-12-07T17:40:26.155069</t>
   </si>
   <si>
-    <t>http://datos.jus.gob.ar/dataset/magistrados-justicia-federal-y-de-la-justicia-nacional/archivo/551c8132-4aef-419a-8f7b-020bb613980b
-</t>
+    <t>http://datos.jus.gob.ar/dataset/magistrados-justicia-federal-y-de-la-justicia-nacional/archivo/551c8132-4aef-419a-8f7b-020bb613980b</t>
   </si>
   <si>
     <t>Renuncia de jueces, fiscales y defensores de la Justicia Federal y de la Justicia Nacional</t>
@@ -1783,8 +1738,7 @@
     <t>2016-12-07T17:41:49.776250</t>
   </si>
   <si>
-    <t>http://datos.jus.gob.ar/dataset/mediaciones-prejudiciales-y-judiciales/archivo/fee87e15-3d5b-4d30-a29f-2dd8815fc015
-</t>
+    <t>http://datos.jus.gob.ar/dataset/mediaciones-prejudiciales-y-judiciales/archivo/fee87e15-3d5b-4d30-a29f-2dd8815fc015</t>
   </si>
   <si>
     <t>Estadística de mediaciones prejudiciales y judiciales efectuadas desde febrero de 2014</t>
@@ -1799,8 +1753,7 @@
     <t>2016-12-05T17:08:12.273577</t>
   </si>
   <si>
-    <t>http://datos.jus.gob.ar/dataset/registro-sistematizacion-y-seguimiento-de-femicidios-y-homicidios-agravados-por-el-genero/archivo/9a06c428-8552-42fe-86e1-487bca9b712c
-</t>
+    <t>http://datos.jus.gob.ar/dataset/registro-sistematizacion-y-seguimiento-de-femicidios-y-homicidios-agravados-por-el-genero/archivo/9a06c428-8552-42fe-86e1-487bca9b712c</t>
   </si>
   <si>
     <t>Esta base registra los femicidios y homicidios agravados por el género desde el año 2012 a la fecha.</t>
@@ -1818,8 +1771,7 @@
     <t>2016-10-28T15:13:12.032921</t>
   </si>
   <si>
-    <t>http://datos.jus.gob.ar/dataset/registro-unificado-de-victimas-del-terrorismo-de-estado-ruvte/archivo/c6b674bc-e178-41f3-81f5-0f10038e1688
-</t>
+    <t>http://datos.jus.gob.ar/dataset/registro-unificado-de-victimas-del-terrorismo-de-estado-ruvte/archivo/c6b674bc-e178-41f3-81f5-0f10038e1688</t>
   </si>
   <si>
     <t>Listado de víctimas del accionar represivo ilegal del Estado argentino entre 1966 y 1983 (víctimas de desaparición forzada y de asesinato).</t>
@@ -1855,8 +1807,7 @@
     <t>2016-11-02T13:22:17.264897</t>
   </si>
   <si>
-    <t>http://datos.jus.gob.ar/dataset/sneep/archivo/b2c3f47c-b78d-4967-98be-0ab81dd0b415
-</t>
+    <t>http://datos.jus.gob.ar/dataset/sneep/archivo/b2c3f47c-b78d-4967-98be-0ab81dd0b415</t>
   </si>
   <si>
     <t>Sistema Nacional de Estadísticas sobre Ejecución de la Pena correspondiente al año 2015</t>
@@ -1874,8 +1825,7 @@
     <t>2016-12-06T14:26:36.775736</t>
   </si>
   <si>
-    <t>http://datos.jus.gob.ar/dataset/sneep/archivo/ae511208-8678-45ac-b088-6b2dd5964f4e
-</t>
+    <t>http://datos.jus.gob.ar/dataset/sneep/archivo/ae511208-8678-45ac-b088-6b2dd5964f4e</t>
   </si>
   <si>
     <t>Sistema Nacional de Estadísticas sobre Ejecución de la Pena correspondiente al año 2014</t>
@@ -1893,8 +1843,7 @@
     <t>2016-12-06T13:08:23.171421</t>
   </si>
   <si>
-    <t>http://datos.jus.gob.ar/dataset/sneep/archivo/f39839a0-cd4a-47a9-bb30-dba81ae61cae
-</t>
+    <t>http://datos.jus.gob.ar/dataset/sneep/archivo/f39839a0-cd4a-47a9-bb30-dba81ae61cae</t>
   </si>
   <si>
     <t>Sistema Nacional de Estadísticas sobre Ejecución de la Pena correspondiente al año 2013</t>
@@ -1912,8 +1861,7 @@
     <t>2016-12-06T15:17:18.345712</t>
   </si>
   <si>
-    <t>http://datos.jus.gob.ar/dataset/sneep/archivo/e289393f-4bfa-49af-8ba2-dbe64a9ba303
-</t>
+    <t>http://datos.jus.gob.ar/dataset/sneep/archivo/e289393f-4bfa-49af-8ba2-dbe64a9ba303</t>
   </si>
   <si>
     <t>Sistema Nacional de Estadísticas sobre Ejecución de la Pena correspondiente al año 2012</t>
@@ -1931,8 +1879,7 @@
     <t>2016-12-07T11:16:54.299344</t>
   </si>
   <si>
-    <t>http://datos.jus.gob.ar/dataset/sneep/archivo/0b5cf2e0-de16-4b71-b3c1-99aeb63d8165
-</t>
+    <t>http://datos.jus.gob.ar/dataset/sneep/archivo/0b5cf2e0-de16-4b71-b3c1-99aeb63d8165</t>
   </si>
   <si>
     <t>Sistema Nacional de Estadísticas sobre Ejecución de la Pena correspondiente al año 2011</t>
@@ -1950,8 +1897,7 @@
     <t>2016-12-06T15:06:55.029084</t>
   </si>
   <si>
-    <t>http://datos.jus.gob.ar/dataset/sneep/archivo/ed1061a5-3d28-4664-82a4-2406231cc0c8
-</t>
+    <t>http://datos.jus.gob.ar/dataset/sneep/archivo/ed1061a5-3d28-4664-82a4-2406231cc0c8</t>
   </si>
   <si>
     <t>Sistema Nacional de Estadísticas sobre Ejecución de la Pena correspondiente al año 2010</t>
@@ -1969,8 +1915,7 @@
     <t>2016-12-06T15:09:15.457540</t>
   </si>
   <si>
-    <t>http://datos.jus.gob.ar/dataset/sneep/archivo/e8cc11d5-0c05-4958-a791-26005adc9562
-</t>
+    <t>http://datos.jus.gob.ar/dataset/sneep/archivo/e8cc11d5-0c05-4958-a791-26005adc9562</t>
   </si>
   <si>
     <t>Sistema Nacional de Estadísticas sobre Ejecución de la Pena correspondiente al año 2009</t>
@@ -1988,8 +1933,7 @@
     <t>2016-12-06T15:56:13.943542</t>
   </si>
   <si>
-    <t>http://datos.jus.gob.ar/dataset/sneep/archivo/f627e52e-e55c-4d7f-bb0b-034a474479a9
-</t>
+    <t>http://datos.jus.gob.ar/dataset/sneep/archivo/f627e52e-e55c-4d7f-bb0b-034a474479a9</t>
   </si>
   <si>
     <t>Sistema Nacional de Estadísticas sobre Ejecución de la Pena correspondiente al año 2008</t>
@@ -2007,8 +1951,7 @@
     <t>2016-12-07T12:20:01.481411</t>
   </si>
   <si>
-    <t>http://datos.jus.gob.ar/dataset/sneep/archivo/d47a67c0-63d7-411d-bd32-19957776f31f
-</t>
+    <t>http://datos.jus.gob.ar/dataset/sneep/archivo/d47a67c0-63d7-411d-bd32-19957776f31f</t>
   </si>
   <si>
     <t>Sistema Nacional de Estadísticas sobre Ejecución de la Pena correspondiente al año 2007</t>
@@ -2026,8 +1969,7 @@
     <t>2016-12-06T16:04:00.383514</t>
   </si>
   <si>
-    <t>http://datos.jus.gob.ar/dataset/sneep/archivo/4315c359-3c3e-429e-bac6-4ae75dad6965
-</t>
+    <t>http://datos.jus.gob.ar/dataset/sneep/archivo/4315c359-3c3e-429e-bac6-4ae75dad6965</t>
   </si>
   <si>
     <t>Sistema Nacional de Estadísticas sobre Ejecución de la Pena correspondiente al año 2006</t>
@@ -2045,8 +1987,7 @@
     <t>2016-12-06T16:05:22.720987</t>
   </si>
   <si>
-    <t>http://datos.jus.gob.ar/dataset/sneep/archivo/81209a1c-782e-4e65-b04c-2bcb39f9c316
-</t>
+    <t>http://datos.jus.gob.ar/dataset/sneep/archivo/81209a1c-782e-4e65-b04c-2bcb39f9c316</t>
   </si>
   <si>
     <t>Sistema Nacional de Estadísticas sobre Ejecución de la Pena correspondiente al año 2005</t>
@@ -2064,8 +2005,7 @@
     <t>2016-12-07T11:18:22.729648</t>
   </si>
   <si>
-    <t>http://datos.jus.gob.ar/dataset/sneep/archivo/124e804b-98c1-4460-ae6a-c392eb7b21a5
-</t>
+    <t>http://datos.jus.gob.ar/dataset/sneep/archivo/124e804b-98c1-4460-ae6a-c392eb7b21a5</t>
   </si>
   <si>
     <t>Sistema Nacional de Estadísticas sobre Ejecución de la Pena correspondiente al año 2004</t>
@@ -2083,8 +2023,7 @@
     <t>2016-12-07T11:34:57.975814</t>
   </si>
   <si>
-    <t>http://datos.jus.gob.ar/dataset/sneep/archivo/a1170dc3-2c57-4b80-bf7a-438cfc3beefd
-</t>
+    <t>http://datos.jus.gob.ar/dataset/sneep/archivo/a1170dc3-2c57-4b80-bf7a-438cfc3beefd</t>
   </si>
   <si>
     <t>Sistema Nacional de Estadísticas sobre Ejecución de la Pena correspondiente al año 2003</t>
@@ -2102,8 +2041,7 @@
     <t>2016-12-07T12:20:32.267502</t>
   </si>
   <si>
-    <t>http://datos.jus.gob.ar/dataset/sneep/archivo/0c05bf5b-e547-42bf-8518-9a80a2ea1b45
-</t>
+    <t>http://datos.jus.gob.ar/dataset/sneep/archivo/0c05bf5b-e547-42bf-8518-9a80a2ea1b45</t>
   </si>
   <si>
     <t>Sistema Nacional de Estadísticas sobre Ejecución de la Pena correspondiente al año 2002</t>
@@ -2121,8 +2059,7 @@
     <t>2016-12-07T12:21:37.859378</t>
   </si>
   <si>
-    <t>http://datos.jus.gob.ar/dataset/solicitudes-condicion-legitimo-usuario-armas-fuego/archivo/0ecec60a-0723-4232-a401-6565ebb282cf
-</t>
+    <t>http://datos.jus.gob.ar/dataset/solicitudes-condicion-legitimo-usuario-armas-fuego/archivo/0ecec60a-0723-4232-a401-6565ebb282cf</t>
   </si>
   <si>
     <t>Listado de Solicitudes de Condición de Legítimo Usuario de Armas de Fuego comprendidas en el "Sistema de Control Ciudadano para Autorizaciones"</t>
@@ -2137,8 +2074,7 @@
     <t>2016-12-16T11:47:01.707897</t>
   </si>
   <si>
-    <t>http://datos.jus.gob.ar/dataset/solicitudes-de-autorizacion-de-portacion-de-armas-de-fuego/archivo/2e0a4e06-0d2e-4e78-861d-1105e558e493
-</t>
+    <t>http://datos.jus.gob.ar/dataset/solicitudes-de-autorizacion-de-portacion-de-armas-de-fuego/archivo/2e0a4e06-0d2e-4e78-861d-1105e558e493</t>
   </si>
   <si>
     <t>Listado de Solicitudes de Autorización de Portación de Armas de Fuego comprendidas en el "Sistema de Control Ciudadano para Autorizaciones".</t>
@@ -2153,8 +2089,7 @@
     <t>2016-12-16T11:48:39.776623</t>
   </si>
   <si>
-    <t>http://datos.jus.gob.ar/dataset/unidad-de-registro-sistematizacion-y-seguimiento-de-hechos-de-violencia-institucional/archivo/56dbd545-f102-4fbd-be48-0edb9b1f846c
-</t>
+    <t>http://datos.jus.gob.ar/dataset/unidad-de-registro-sistematizacion-y-seguimiento-de-hechos-de-violencia-institucional/archivo/56dbd545-f102-4fbd-be48-0edb9b1f846c</t>
   </si>
   <si>
     <t>Seguimientos de hechos de violencia institucional sobre la base de las presentaciones, denuncias e informaciones recibidas en el ámbito de la Secretaría de Derechos Humanos.</t>
@@ -2175,94 +2110,110 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="19">
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
-    <font/>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
     <font>
       <b/>
-      <sz val="9.0"/>
+      <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="9.0"/>
+      <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="8.0"/>
+      <sz val="8"/>
+      <name val="Calibri"/>
     </font>
     <font>
       <b/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
     <font>
-      <sz val="9.0"/>
+      <sz val="9"/>
+      <name val="Calibri"/>
     </font>
     <font>
       <u/>
-      <sz val="8.0"/>
+      <sz val="8"/>
       <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
     </font>
     <font>
       <u/>
-      <sz val="9.0"/>
+      <sz val="9"/>
       <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
     </font>
     <font>
       <b/>
       <i/>
+      <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
     </font>
     <font>
       <b/>
       <i/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
     </font>
     <font>
       <u/>
-      <sz val="9.0"/>
+      <sz val="9"/>
       <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
     </font>
     <font>
-      <sz val="9.0"/>
+      <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
       <b/>
+      <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
     </font>
     <font>
       <u/>
-      <sz val="9.0"/>
+      <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
       <u/>
-      <sz val="9.0"/>
+      <sz val="9"/>
       <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
     </font>
     <font>
-      <sz val="9.0"/>
+      <sz val="9"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
     </font>
     <font>
       <u/>
-      <sz val="9.0"/>
+      <sz val="9"/>
       <color rgb="FF0000FF"/>
       <name val="Calibri"/>
     </font>
@@ -2272,7 +2223,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -2311,6 +2262,7 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -2325,174 +2277,603 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="36">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="5" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="5" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="1" fillId="5" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="5" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="6" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="6" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
-    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1026" name="Rectangle 2" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3074" name="Rectangle 2" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4099" name="Rectangle 3" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>2657475</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2053" name="Rectangle 5" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
-</file>
-
-<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="15.13" defaultRowHeight="15.0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="15.140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="20.5"/>
-    <col customWidth="1" min="2" max="2" width="51.38"/>
-    <col customWidth="1" min="3" max="3" width="22.75"/>
-    <col customWidth="1" min="4" max="4" width="22.13"/>
-    <col customWidth="1" min="5" max="5" width="20.25"/>
-    <col customWidth="1" min="6" max="6" width="16.75"/>
-    <col customWidth="1" min="7" max="7" width="16.63"/>
-    <col customWidth="1" min="8" max="8" width="27.63"/>
-    <col customWidth="1" min="9" max="9" width="20.75"/>
-    <col customWidth="1" min="10" max="10" width="17.38"/>
-    <col customWidth="1" min="11" max="11" width="16.0"/>
-    <col customWidth="1" min="12" max="12" width="23.13"/>
+    <col min="1" max="1" width="20.42578125" customWidth="1"/>
+    <col min="2" max="2" width="51.42578125" customWidth="1"/>
+    <col min="3" max="3" width="22.7109375" customWidth="1"/>
+    <col min="4" max="4" width="22.140625" customWidth="1"/>
+    <col min="5" max="5" width="20.28515625" customWidth="1"/>
+    <col min="6" max="6" width="16.7109375" customWidth="1"/>
+    <col min="7" max="7" width="16.5703125" customWidth="1"/>
+    <col min="8" max="8" width="27.5703125" customWidth="1"/>
+    <col min="9" max="9" width="20.7109375" customWidth="1"/>
+    <col min="10" max="10" width="17.42578125" customWidth="1"/>
+    <col min="11" max="11" width="16" customWidth="1"/>
+    <col min="12" max="12" width="23.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:12">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -2530,7 +2911,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:12">
       <c r="A2" s="6" t="s">
         <v>22</v>
       </c>
@@ -2558,27 +2939,29 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId2" ref="H2"/>
-    <hyperlink r:id="rId3" ref="J2"/>
+    <hyperlink ref="H2" r:id="rId1"/>
+    <hyperlink ref="J2" r:id="rId2"/>
   </hyperlinks>
-  <drawing r:id="rId4"/>
-  <legacyDrawing r:id="rId5"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId3"/>
+  <legacyDrawing r:id="rId4"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="15.13" defaultRowHeight="15.0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="15.140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="17.88"/>
-    <col customWidth="1" min="2" max="2" width="34.0"/>
-    <col customWidth="1" min="3" max="3" width="34.38"/>
+    <col min="1" max="1" width="17.85546875" customWidth="1"/>
+    <col min="2" max="2" width="34" customWidth="1"/>
+    <col min="3" max="3" width="34.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2589,7 +2972,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:3">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
@@ -2600,7 +2983,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:3">
       <c r="A3" s="3" t="s">
         <v>12</v>
       </c>
@@ -2611,7 +2994,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:3">
       <c r="A4" s="3" t="s">
         <v>23</v>
       </c>
@@ -2622,7 +3005,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:3">
       <c r="A5" s="3" t="s">
         <v>26</v>
       </c>
@@ -2633,7 +3016,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:3">
       <c r="A6" s="3" t="s">
         <v>29</v>
       </c>
@@ -2644,7 +3027,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:3">
       <c r="A7" s="3" t="s">
         <v>32</v>
       </c>
@@ -2655,7 +3038,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:3">
       <c r="A8" s="3" t="s">
         <v>35</v>
       </c>
@@ -2666,7 +3049,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:3">
       <c r="A9" s="3" t="s">
         <v>38</v>
       </c>
@@ -2677,7 +3060,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:3">
       <c r="A10" s="3" t="s">
         <v>43</v>
       </c>
@@ -2689,34 +3072,37 @@
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:R23"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="15.13" defaultRowHeight="15.0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="15.140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="30.5"/>
-    <col customWidth="1" min="2" max="2" width="61.0"/>
-    <col customWidth="1" min="3" max="3" width="51.5"/>
-    <col customWidth="1" min="4" max="4" width="34.63"/>
-    <col customWidth="1" min="5" max="5" width="31.75"/>
-    <col customWidth="1" min="6" max="6" width="29.63"/>
-    <col customWidth="1" min="7" max="7" width="23.13"/>
-    <col customWidth="1" min="9" max="9" width="24.13"/>
-    <col customWidth="1" min="10" max="10" width="29.88"/>
-    <col customWidth="1" min="11" max="11" width="26.0"/>
-    <col customWidth="1" min="12" max="12" width="32.0"/>
-    <col customWidth="1" min="13" max="13" width="28.75"/>
-    <col customWidth="1" min="17" max="17" width="30.25"/>
-    <col customWidth="1" min="18" max="18" width="34.13"/>
+    <col min="1" max="1" width="30.42578125" customWidth="1"/>
+    <col min="2" max="2" width="61" customWidth="1"/>
+    <col min="3" max="3" width="51.42578125" customWidth="1"/>
+    <col min="4" max="4" width="34.5703125" customWidth="1"/>
+    <col min="5" max="5" width="31.7109375" customWidth="1"/>
+    <col min="6" max="6" width="29.5703125" customWidth="1"/>
+    <col min="7" max="7" width="23.140625" customWidth="1"/>
+    <col min="9" max="9" width="24.140625" customWidth="1"/>
+    <col min="10" max="10" width="29.85546875" customWidth="1"/>
+    <col min="11" max="11" width="26" customWidth="1"/>
+    <col min="12" max="12" width="32" customWidth="1"/>
+    <col min="13" max="13" width="28.7109375" customWidth="1"/>
+    <col min="17" max="17" width="30.28515625" customWidth="1"/>
+    <col min="18" max="18" width="34.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:18">
       <c r="A1" s="7" t="s">
         <v>2</v>
       </c>
@@ -2772,7 +3158,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:18">
       <c r="A2" s="10" t="s">
         <v>64</v>
       </c>
@@ -2822,7 +3208,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:18">
       <c r="A3" s="10" t="s">
         <v>79</v>
       </c>
@@ -2872,7 +3258,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:18">
       <c r="A4" s="10" t="s">
         <v>89</v>
       </c>
@@ -2922,7 +3308,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:18">
       <c r="A5" s="10" t="s">
         <v>100</v>
       </c>
@@ -2972,7 +3358,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:18">
       <c r="A6" s="19" t="s">
         <v>113</v>
       </c>
@@ -3022,7 +3408,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:18">
       <c r="A7" s="19" t="s">
         <v>132</v>
       </c>
@@ -3072,10 +3458,8 @@
         <v>145</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" s="19" t="s">
-        <v>146</v>
-      </c>
+    <row r="8" spans="1:18">
+      <c r="A8" s="19"/>
       <c r="B8" s="19" t="s">
         <v>147</v>
       </c>
@@ -3118,7 +3502,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:18">
       <c r="A9" s="19" t="s">
         <v>157</v>
       </c>
@@ -3168,7 +3552,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:18">
       <c r="A10" s="19" t="s">
         <v>191</v>
       </c>
@@ -3218,7 +3602,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:18">
       <c r="A11" s="19" t="s">
         <v>216</v>
       </c>
@@ -3268,7 +3652,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:18">
       <c r="A12" s="19" t="s">
         <v>239</v>
       </c>
@@ -3318,7 +3702,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:18">
       <c r="A13" s="19" t="s">
         <v>263</v>
       </c>
@@ -3368,7 +3752,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:18">
       <c r="A14" s="19" t="s">
         <v>284</v>
       </c>
@@ -3418,7 +3802,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:18">
       <c r="A15" s="19" t="s">
         <v>303</v>
       </c>
@@ -3468,7 +3852,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:18">
       <c r="A16" s="19" t="s">
         <v>329</v>
       </c>
@@ -3518,7 +3902,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:18">
       <c r="A17" s="19" t="s">
         <v>348</v>
       </c>
@@ -3568,72 +3952,74 @@
         <v>78</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:18">
       <c r="Q18" s="10"/>
     </row>
-    <row r="19">
+    <row r="19" spans="1:18">
       <c r="Q19" s="10"/>
     </row>
-    <row r="20">
+    <row r="20" spans="1:18">
       <c r="Q20" s="10"/>
     </row>
-    <row r="21">
+    <row r="21" spans="1:18">
       <c r="Q21" s="10"/>
     </row>
-    <row r="22">
+    <row r="22" spans="1:18">
       <c r="Q22" s="10"/>
     </row>
-    <row r="23">
+    <row r="23" spans="1:18">
       <c r="Q23" s="10"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId2" ref="Q2"/>
-    <hyperlink r:id="rId3" ref="Q3"/>
-    <hyperlink r:id="rId4" ref="Q4"/>
-    <hyperlink r:id="rId5" ref="Q5"/>
-    <hyperlink r:id="rId6" ref="Q6"/>
-    <hyperlink r:id="rId7" ref="Q7"/>
-    <hyperlink r:id="rId8" ref="Q8"/>
-    <hyperlink r:id="rId9" ref="Q9"/>
-    <hyperlink r:id="rId10" ref="Q10"/>
-    <hyperlink r:id="rId11" ref="Q11"/>
-    <hyperlink r:id="rId12" ref="Q12"/>
-    <hyperlink r:id="rId13" ref="Q13"/>
-    <hyperlink r:id="rId14" ref="Q14"/>
-    <hyperlink r:id="rId15" ref="Q15"/>
-    <hyperlink r:id="rId16" ref="Q16"/>
-    <hyperlink r:id="rId17" ref="Q17"/>
+    <hyperlink ref="Q2" r:id="rId1"/>
+    <hyperlink ref="Q3" r:id="rId2"/>
+    <hyperlink ref="Q4" r:id="rId3"/>
+    <hyperlink ref="Q5" r:id="rId4"/>
+    <hyperlink ref="Q6" r:id="rId5"/>
+    <hyperlink ref="Q7" r:id="rId6"/>
+    <hyperlink ref="Q8" r:id="rId7"/>
+    <hyperlink ref="Q9" r:id="rId8"/>
+    <hyperlink ref="Q10" r:id="rId9"/>
+    <hyperlink ref="Q11" r:id="rId10"/>
+    <hyperlink ref="Q12" r:id="rId11"/>
+    <hyperlink ref="Q13" r:id="rId12"/>
+    <hyperlink ref="Q14" r:id="rId13"/>
+    <hyperlink ref="Q15" r:id="rId14"/>
+    <hyperlink ref="Q16" r:id="rId15"/>
+    <hyperlink ref="Q17" r:id="rId16"/>
   </hyperlinks>
-  <drawing r:id="rId18"/>
-  <legacyDrawing r:id="rId19"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId17"/>
+  <legacyDrawing r:id="rId18"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="15.13" defaultRowHeight="15.0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="15.140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="30.75"/>
-    <col customWidth="1" min="2" max="2" width="36.75"/>
-    <col customWidth="1" min="3" max="3" width="70.25"/>
-    <col customWidth="1" min="4" max="4" width="59.13"/>
-    <col customWidth="1" min="5" max="5" width="16.88"/>
-    <col customWidth="1" min="6" max="6" width="19.38"/>
-    <col customWidth="1" min="7" max="7" width="70.75"/>
-    <col customWidth="1" min="8" max="8" width="37.0"/>
-    <col customWidth="1" min="10" max="10" width="20.38"/>
-    <col customWidth="1" min="11" max="11" width="23.25"/>
-    <col customWidth="1" min="12" max="12" width="27.63"/>
+    <col min="1" max="1" width="30.7109375" customWidth="1"/>
+    <col min="2" max="2" width="36.7109375" customWidth="1"/>
+    <col min="3" max="3" width="70.28515625" customWidth="1"/>
+    <col min="4" max="4" width="59.140625" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" customWidth="1"/>
+    <col min="6" max="6" width="19.42578125" customWidth="1"/>
+    <col min="7" max="7" width="70.7109375" customWidth="1"/>
+    <col min="8" max="8" width="37" customWidth="1"/>
+    <col min="10" max="10" width="20.42578125" customWidth="1"/>
+    <col min="11" max="11" width="23.28515625" customWidth="1"/>
+    <col min="12" max="12" width="27.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:13">
       <c r="A1" s="14" t="s">
         <v>58</v>
       </c>
@@ -3674,7 +4060,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:13">
       <c r="A2" s="22" t="s">
         <v>75</v>
       </c>
@@ -3707,7 +4093,7 @@
       </c>
       <c r="M2" s="28"/>
     </row>
-    <row r="3">
+    <row r="3" spans="1:13">
       <c r="A3" s="22" t="s">
         <v>162</v>
       </c>
@@ -3740,7 +4126,7 @@
       </c>
       <c r="M3" s="28"/>
     </row>
-    <row r="4">
+    <row r="4" spans="1:13">
       <c r="A4" s="22" t="s">
         <v>162</v>
       </c>
@@ -3773,7 +4159,7 @@
       </c>
       <c r="M4" s="28"/>
     </row>
-    <row r="5">
+    <row r="5" spans="1:13">
       <c r="A5" s="24" t="s">
         <v>87</v>
       </c>
@@ -3806,7 +4192,7 @@
       </c>
       <c r="M5" s="28"/>
     </row>
-    <row r="6">
+    <row r="6" spans="1:13">
       <c r="A6" s="24" t="s">
         <v>98</v>
       </c>
@@ -3839,7 +4225,7 @@
       </c>
       <c r="M6" s="28"/>
     </row>
-    <row r="7">
+    <row r="7" spans="1:13">
       <c r="A7" s="24" t="s">
         <v>110</v>
       </c>
@@ -3872,7 +4258,7 @@
       </c>
       <c r="M7" s="28"/>
     </row>
-    <row r="8">
+    <row r="8" spans="1:13">
       <c r="A8" s="24" t="s">
         <v>110</v>
       </c>
@@ -3905,7 +4291,7 @@
       </c>
       <c r="M8" s="28"/>
     </row>
-    <row r="9">
+    <row r="9" spans="1:13">
       <c r="A9" s="24" t="s">
         <v>110</v>
       </c>
@@ -3938,7 +4324,7 @@
       </c>
       <c r="M9" s="28"/>
     </row>
-    <row r="10">
+    <row r="10" spans="1:13">
       <c r="A10" s="31" t="s">
         <v>291</v>
       </c>
@@ -3971,7 +4357,7 @@
       </c>
       <c r="M10" s="28"/>
     </row>
-    <row r="11">
+    <row r="11" spans="1:13">
       <c r="A11" s="31" t="s">
         <v>129</v>
       </c>
@@ -4004,7 +4390,7 @@
       </c>
       <c r="M11" s="28"/>
     </row>
-    <row r="12">
+    <row r="12" spans="1:13">
       <c r="A12" s="31" t="s">
         <v>129</v>
       </c>
@@ -4037,7 +4423,7 @@
       </c>
       <c r="M12" s="28"/>
     </row>
-    <row r="13">
+    <row r="13" spans="1:13">
       <c r="A13" s="31" t="s">
         <v>129</v>
       </c>
@@ -4070,7 +4456,7 @@
       </c>
       <c r="M13" s="28"/>
     </row>
-    <row r="14">
+    <row r="14" spans="1:13">
       <c r="A14" s="31" t="s">
         <v>129</v>
       </c>
@@ -4103,7 +4489,7 @@
       </c>
       <c r="M14" s="28"/>
     </row>
-    <row r="15">
+    <row r="15" spans="1:13">
       <c r="A15" s="31" t="s">
         <v>129</v>
       </c>
@@ -4136,7 +4522,7 @@
       </c>
       <c r="M15" s="28"/>
     </row>
-    <row r="16">
+    <row r="16" spans="1:13">
       <c r="A16" s="31" t="s">
         <v>129</v>
       </c>
@@ -4169,7 +4555,7 @@
       </c>
       <c r="M16" s="28"/>
     </row>
-    <row r="17">
+    <row r="17" spans="1:13">
       <c r="A17" s="31" t="s">
         <v>129</v>
       </c>
@@ -4202,7 +4588,7 @@
       </c>
       <c r="M17" s="28"/>
     </row>
-    <row r="18">
+    <row r="18" spans="1:13">
       <c r="A18" s="31" t="s">
         <v>129</v>
       </c>
@@ -4235,7 +4621,7 @@
       </c>
       <c r="M18" s="28"/>
     </row>
-    <row r="19">
+    <row r="19" spans="1:13">
       <c r="A19" s="31" t="s">
         <v>129</v>
       </c>
@@ -4268,7 +4654,7 @@
       </c>
       <c r="M19" s="28"/>
     </row>
-    <row r="20">
+    <row r="20" spans="1:13">
       <c r="A20" s="31" t="s">
         <v>129</v>
       </c>
@@ -4301,7 +4687,7 @@
       </c>
       <c r="M20" s="28"/>
     </row>
-    <row r="21">
+    <row r="21" spans="1:13">
       <c r="A21" s="31" t="s">
         <v>129</v>
       </c>
@@ -4334,7 +4720,7 @@
       </c>
       <c r="M21" s="28"/>
     </row>
-    <row r="22">
+    <row r="22" spans="1:13">
       <c r="A22" s="31" t="s">
         <v>129</v>
       </c>
@@ -4367,7 +4753,7 @@
       </c>
       <c r="M22" s="28"/>
     </row>
-    <row r="23">
+    <row r="23" spans="1:13">
       <c r="A23" s="31" t="s">
         <v>129</v>
       </c>
@@ -4400,7 +4786,7 @@
       </c>
       <c r="M23" s="28"/>
     </row>
-    <row r="24">
+    <row r="24" spans="1:13">
       <c r="A24" s="31" t="s">
         <v>129</v>
       </c>
@@ -4433,7 +4819,7 @@
       </c>
       <c r="M24" s="28"/>
     </row>
-    <row r="25">
+    <row r="25" spans="1:13">
       <c r="A25" s="31" t="s">
         <v>129</v>
       </c>
@@ -4466,7 +4852,7 @@
       </c>
       <c r="M25" s="28"/>
     </row>
-    <row r="26">
+    <row r="26" spans="1:13">
       <c r="A26" s="31" t="s">
         <v>141</v>
       </c>
@@ -4499,7 +4885,7 @@
       </c>
       <c r="M26" s="28"/>
     </row>
-    <row r="27">
+    <row r="27" spans="1:13">
       <c r="A27" s="31" t="s">
         <v>154</v>
       </c>
@@ -4532,7 +4918,7 @@
       </c>
       <c r="M27" s="28"/>
     </row>
-    <row r="28">
+    <row r="28" spans="1:13">
       <c r="A28" s="31" t="s">
         <v>154</v>
       </c>
@@ -4565,7 +4951,7 @@
       </c>
       <c r="M28" s="28"/>
     </row>
-    <row r="29">
+    <row r="29" spans="1:13">
       <c r="A29" s="31" t="s">
         <v>154</v>
       </c>
@@ -4598,7 +4984,7 @@
       </c>
       <c r="M29" s="28"/>
     </row>
-    <row r="30">
+    <row r="30" spans="1:13">
       <c r="A30" s="31" t="s">
         <v>154</v>
       </c>
@@ -4631,7 +5017,7 @@
       </c>
       <c r="M30" s="28"/>
     </row>
-    <row r="31">
+    <row r="31" spans="1:13">
       <c r="A31" s="31" t="s">
         <v>154</v>
       </c>
@@ -4664,7 +5050,7 @@
       </c>
       <c r="M31" s="28"/>
     </row>
-    <row r="32">
+    <row r="32" spans="1:13">
       <c r="A32" s="31" t="s">
         <v>154</v>
       </c>
@@ -4697,7 +5083,7 @@
       </c>
       <c r="M32" s="28"/>
     </row>
-    <row r="33">
+    <row r="33" spans="1:13">
       <c r="A33" s="31" t="s">
         <v>177</v>
       </c>
@@ -4730,7 +5116,7 @@
       </c>
       <c r="M33" s="28"/>
     </row>
-    <row r="34">
+    <row r="34" spans="1:13">
       <c r="A34" s="31" t="s">
         <v>209</v>
       </c>
@@ -4763,7 +5149,7 @@
       </c>
       <c r="M34" s="28"/>
     </row>
-    <row r="35">
+    <row r="35" spans="1:13">
       <c r="A35" s="31" t="s">
         <v>209</v>
       </c>
@@ -4796,7 +5182,7 @@
       </c>
       <c r="M35" s="28"/>
     </row>
-    <row r="36">
+    <row r="36" spans="1:13">
       <c r="A36" s="31" t="s">
         <v>209</v>
       </c>
@@ -4829,7 +5215,7 @@
       </c>
       <c r="M36" s="28"/>
     </row>
-    <row r="37">
+    <row r="37" spans="1:13">
       <c r="A37" s="31" t="s">
         <v>232</v>
       </c>
@@ -4862,7 +5248,7 @@
       </c>
       <c r="M37" s="28"/>
     </row>
-    <row r="38">
+    <row r="38" spans="1:13">
       <c r="A38" s="31" t="s">
         <v>256</v>
       </c>
@@ -4895,7 +5281,7 @@
       </c>
       <c r="M38" s="28"/>
     </row>
-    <row r="39">
+    <row r="39" spans="1:13">
       <c r="A39" s="31" t="s">
         <v>278</v>
       </c>
@@ -4928,7 +5314,7 @@
       </c>
       <c r="M39" s="28"/>
     </row>
-    <row r="40">
+    <row r="40" spans="1:13">
       <c r="A40" s="31" t="s">
         <v>278</v>
       </c>
@@ -4961,7 +5347,7 @@
       </c>
       <c r="M40" s="28"/>
     </row>
-    <row r="41">
+    <row r="41" spans="1:13">
       <c r="A41" s="31" t="s">
         <v>298</v>
       </c>
@@ -4994,7 +5380,7 @@
       </c>
       <c r="M41" s="28"/>
     </row>
-    <row r="42">
+    <row r="42" spans="1:13">
       <c r="A42" s="31" t="s">
         <v>298</v>
       </c>
@@ -5027,7 +5413,7 @@
       </c>
       <c r="M42" s="28"/>
     </row>
-    <row r="43">
+    <row r="43" spans="1:13">
       <c r="A43" s="31" t="s">
         <v>298</v>
       </c>
@@ -5060,7 +5446,7 @@
       </c>
       <c r="M43" s="28"/>
     </row>
-    <row r="44">
+    <row r="44" spans="1:13">
       <c r="A44" s="31" t="s">
         <v>298</v>
       </c>
@@ -5093,7 +5479,7 @@
       </c>
       <c r="M44" s="28"/>
     </row>
-    <row r="45">
+    <row r="45" spans="1:13">
       <c r="A45" s="31" t="s">
         <v>298</v>
       </c>
@@ -5126,7 +5512,7 @@
       </c>
       <c r="M45" s="28"/>
     </row>
-    <row r="46">
+    <row r="46" spans="1:13">
       <c r="A46" s="31" t="s">
         <v>298</v>
       </c>
@@ -5159,7 +5545,7 @@
       </c>
       <c r="M46" s="28"/>
     </row>
-    <row r="47">
+    <row r="47" spans="1:13">
       <c r="A47" s="31" t="s">
         <v>298</v>
       </c>
@@ -5192,7 +5578,7 @@
       </c>
       <c r="M47" s="28"/>
     </row>
-    <row r="48">
+    <row r="48" spans="1:13">
       <c r="A48" s="31" t="s">
         <v>298</v>
       </c>
@@ -5225,7 +5611,7 @@
       </c>
       <c r="M48" s="28"/>
     </row>
-    <row r="49">
+    <row r="49" spans="1:13">
       <c r="A49" s="31" t="s">
         <v>298</v>
       </c>
@@ -5258,7 +5644,7 @@
       </c>
       <c r="M49" s="28"/>
     </row>
-    <row r="50">
+    <row r="50" spans="1:13">
       <c r="A50" s="31" t="s">
         <v>298</v>
       </c>
@@ -5291,7 +5677,7 @@
       </c>
       <c r="M50" s="28"/>
     </row>
-    <row r="51">
+    <row r="51" spans="1:13">
       <c r="A51" s="31" t="s">
         <v>298</v>
       </c>
@@ -5324,7 +5710,7 @@
       </c>
       <c r="M51" s="28"/>
     </row>
-    <row r="52">
+    <row r="52" spans="1:13">
       <c r="A52" s="31" t="s">
         <v>298</v>
       </c>
@@ -5357,7 +5743,7 @@
       </c>
       <c r="M52" s="28"/>
     </row>
-    <row r="53">
+    <row r="53" spans="1:13">
       <c r="A53" s="31" t="s">
         <v>298</v>
       </c>
@@ -5390,7 +5776,7 @@
       </c>
       <c r="M53" s="28"/>
     </row>
-    <row r="54">
+    <row r="54" spans="1:13">
       <c r="A54" s="31" t="s">
         <v>298</v>
       </c>
@@ -5423,7 +5809,7 @@
       </c>
       <c r="M54" s="28"/>
     </row>
-    <row r="55">
+    <row r="55" spans="1:13">
       <c r="A55" s="31" t="s">
         <v>323</v>
       </c>
@@ -5456,7 +5842,7 @@
       </c>
       <c r="M55" s="28"/>
     </row>
-    <row r="56">
+    <row r="56" spans="1:13">
       <c r="A56" s="31" t="s">
         <v>340</v>
       </c>
@@ -5489,7 +5875,7 @@
       </c>
       <c r="M56" s="28"/>
     </row>
-    <row r="57">
+    <row r="57" spans="1:13">
       <c r="A57" s="31" t="s">
         <v>364</v>
       </c>
@@ -5524,142 +5910,144 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId2" ref="C2"/>
-    <hyperlink r:id="rId3" ref="G2"/>
-    <hyperlink r:id="rId4" ref="C3"/>
-    <hyperlink r:id="rId5" ref="G3"/>
-    <hyperlink r:id="rId6" ref="C4"/>
-    <hyperlink r:id="rId7" ref="G4"/>
-    <hyperlink r:id="rId8" ref="C5"/>
-    <hyperlink r:id="rId9" ref="G5"/>
-    <hyperlink r:id="rId10" ref="C6"/>
-    <hyperlink r:id="rId11" ref="G6"/>
-    <hyperlink r:id="rId12" ref="C7"/>
-    <hyperlink r:id="rId13" ref="G7"/>
-    <hyperlink r:id="rId14" ref="C8"/>
-    <hyperlink r:id="rId15" ref="G8"/>
-    <hyperlink r:id="rId16" ref="C9"/>
-    <hyperlink r:id="rId17" ref="G9"/>
-    <hyperlink r:id="rId18" ref="C10"/>
-    <hyperlink r:id="rId19" ref="G10"/>
-    <hyperlink r:id="rId20" ref="C11"/>
-    <hyperlink r:id="rId21" ref="G11"/>
-    <hyperlink r:id="rId22" ref="C12"/>
-    <hyperlink r:id="rId23" ref="G12"/>
-    <hyperlink r:id="rId24" ref="C13"/>
-    <hyperlink r:id="rId25" ref="G13"/>
-    <hyperlink r:id="rId26" ref="C14"/>
-    <hyperlink r:id="rId27" ref="G14"/>
-    <hyperlink r:id="rId28" ref="C15"/>
-    <hyperlink r:id="rId29" ref="G15"/>
-    <hyperlink r:id="rId30" ref="C16"/>
-    <hyperlink r:id="rId31" ref="G16"/>
-    <hyperlink r:id="rId32" ref="C17"/>
-    <hyperlink r:id="rId33" ref="G17"/>
-    <hyperlink r:id="rId34" ref="C18"/>
-    <hyperlink r:id="rId35" ref="G18"/>
-    <hyperlink r:id="rId36" ref="C19"/>
-    <hyperlink r:id="rId37" ref="G19"/>
-    <hyperlink r:id="rId38" ref="C20"/>
-    <hyperlink r:id="rId39" ref="G20"/>
-    <hyperlink r:id="rId40" ref="C21"/>
-    <hyperlink r:id="rId41" ref="G21"/>
-    <hyperlink r:id="rId42" ref="C22"/>
-    <hyperlink r:id="rId43" ref="G22"/>
-    <hyperlink r:id="rId44" ref="C23"/>
-    <hyperlink r:id="rId45" ref="G23"/>
-    <hyperlink r:id="rId46" ref="C24"/>
-    <hyperlink r:id="rId47" ref="G24"/>
-    <hyperlink r:id="rId48" ref="C25"/>
-    <hyperlink r:id="rId49" ref="G25"/>
-    <hyperlink r:id="rId50" ref="C26"/>
-    <hyperlink r:id="rId51" ref="G26"/>
-    <hyperlink r:id="rId52" ref="C27"/>
-    <hyperlink r:id="rId53" ref="G27"/>
-    <hyperlink r:id="rId54" ref="C28"/>
-    <hyperlink r:id="rId55" ref="G28"/>
-    <hyperlink r:id="rId56" ref="C29"/>
-    <hyperlink r:id="rId57" ref="G29"/>
-    <hyperlink r:id="rId58" ref="C30"/>
-    <hyperlink r:id="rId59" ref="G30"/>
-    <hyperlink r:id="rId60" ref="C31"/>
-    <hyperlink r:id="rId61" ref="G31"/>
-    <hyperlink r:id="rId62" ref="C32"/>
-    <hyperlink r:id="rId63" ref="G32"/>
-    <hyperlink r:id="rId64" ref="C33"/>
-    <hyperlink r:id="rId65" ref="G33"/>
-    <hyperlink r:id="rId66" ref="C34"/>
-    <hyperlink r:id="rId67" ref="G34"/>
-    <hyperlink r:id="rId68" ref="C35"/>
-    <hyperlink r:id="rId69" ref="G35"/>
-    <hyperlink r:id="rId70" ref="C36"/>
-    <hyperlink r:id="rId71" ref="G36"/>
-    <hyperlink r:id="rId72" ref="C37"/>
-    <hyperlink r:id="rId73" ref="G37"/>
-    <hyperlink r:id="rId74" ref="C38"/>
-    <hyperlink r:id="rId75" ref="G38"/>
-    <hyperlink r:id="rId76" ref="C39"/>
-    <hyperlink r:id="rId77" ref="G39"/>
-    <hyperlink r:id="rId78" ref="C40"/>
-    <hyperlink r:id="rId79" ref="G40"/>
-    <hyperlink r:id="rId80" ref="C41"/>
-    <hyperlink r:id="rId81" ref="G41"/>
-    <hyperlink r:id="rId82" ref="C42"/>
-    <hyperlink r:id="rId83" ref="G42"/>
-    <hyperlink r:id="rId84" ref="C43"/>
-    <hyperlink r:id="rId85" ref="G43"/>
-    <hyperlink r:id="rId86" ref="C44"/>
-    <hyperlink r:id="rId87" ref="G44"/>
-    <hyperlink r:id="rId88" ref="C45"/>
-    <hyperlink r:id="rId89" ref="G45"/>
-    <hyperlink r:id="rId90" ref="C46"/>
-    <hyperlink r:id="rId91" ref="G46"/>
-    <hyperlink r:id="rId92" ref="C47"/>
-    <hyperlink r:id="rId93" ref="G47"/>
-    <hyperlink r:id="rId94" ref="C48"/>
-    <hyperlink r:id="rId95" ref="G48"/>
-    <hyperlink r:id="rId96" ref="C49"/>
-    <hyperlink r:id="rId97" ref="G49"/>
-    <hyperlink r:id="rId98" ref="C50"/>
-    <hyperlink r:id="rId99" ref="G50"/>
-    <hyperlink r:id="rId100" ref="C51"/>
-    <hyperlink r:id="rId101" ref="G51"/>
-    <hyperlink r:id="rId102" ref="C52"/>
-    <hyperlink r:id="rId103" ref="G52"/>
-    <hyperlink r:id="rId104" ref="C53"/>
-    <hyperlink r:id="rId105" ref="G53"/>
-    <hyperlink r:id="rId106" ref="C54"/>
-    <hyperlink r:id="rId107" ref="G54"/>
-    <hyperlink r:id="rId108" ref="C55"/>
-    <hyperlink r:id="rId109" ref="G55"/>
-    <hyperlink r:id="rId110" ref="C56"/>
-    <hyperlink r:id="rId111" ref="G56"/>
-    <hyperlink r:id="rId112" ref="C57"/>
-    <hyperlink r:id="rId113" ref="G57"/>
+    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="G2" r:id="rId2"/>
+    <hyperlink ref="C3" r:id="rId3"/>
+    <hyperlink ref="G3" r:id="rId4"/>
+    <hyperlink ref="C4" r:id="rId5"/>
+    <hyperlink ref="G4" r:id="rId6"/>
+    <hyperlink ref="C5" r:id="rId7"/>
+    <hyperlink ref="G5" r:id="rId8"/>
+    <hyperlink ref="C6" r:id="rId9"/>
+    <hyperlink ref="G6" r:id="rId10"/>
+    <hyperlink ref="C7" r:id="rId11"/>
+    <hyperlink ref="G7" r:id="rId12"/>
+    <hyperlink ref="C8" r:id="rId13"/>
+    <hyperlink ref="G8" r:id="rId14"/>
+    <hyperlink ref="C9" r:id="rId15"/>
+    <hyperlink ref="G9" r:id="rId16"/>
+    <hyperlink ref="C10" r:id="rId17"/>
+    <hyperlink ref="G10" r:id="rId18"/>
+    <hyperlink ref="C11" r:id="rId19"/>
+    <hyperlink ref="G11" r:id="rId20"/>
+    <hyperlink ref="C12" r:id="rId21"/>
+    <hyperlink ref="G12" r:id="rId22"/>
+    <hyperlink ref="C13" r:id="rId23"/>
+    <hyperlink ref="G13" r:id="rId24"/>
+    <hyperlink ref="C14" r:id="rId25"/>
+    <hyperlink ref="G14" r:id="rId26"/>
+    <hyperlink ref="C15" r:id="rId27"/>
+    <hyperlink ref="G15" r:id="rId28"/>
+    <hyperlink ref="C16" r:id="rId29"/>
+    <hyperlink ref="G16" r:id="rId30"/>
+    <hyperlink ref="C17" r:id="rId31"/>
+    <hyperlink ref="G17" r:id="rId32"/>
+    <hyperlink ref="C18" r:id="rId33"/>
+    <hyperlink ref="G18" r:id="rId34"/>
+    <hyperlink ref="C19" r:id="rId35"/>
+    <hyperlink ref="G19" r:id="rId36"/>
+    <hyperlink ref="C20" r:id="rId37"/>
+    <hyperlink ref="G20" r:id="rId38"/>
+    <hyperlink ref="C21" r:id="rId39"/>
+    <hyperlink ref="G21" r:id="rId40"/>
+    <hyperlink ref="C22" r:id="rId41"/>
+    <hyperlink ref="G22" r:id="rId42"/>
+    <hyperlink ref="C23" r:id="rId43"/>
+    <hyperlink ref="G23" r:id="rId44"/>
+    <hyperlink ref="C24" r:id="rId45"/>
+    <hyperlink ref="G24" r:id="rId46"/>
+    <hyperlink ref="C25" r:id="rId47"/>
+    <hyperlink ref="G25" r:id="rId48"/>
+    <hyperlink ref="C26" r:id="rId49"/>
+    <hyperlink ref="G26" r:id="rId50"/>
+    <hyperlink ref="C27" r:id="rId51"/>
+    <hyperlink ref="G27" r:id="rId52"/>
+    <hyperlink ref="C28" r:id="rId53"/>
+    <hyperlink ref="G28" r:id="rId54"/>
+    <hyperlink ref="C29" r:id="rId55"/>
+    <hyperlink ref="G29" r:id="rId56"/>
+    <hyperlink ref="C30" r:id="rId57"/>
+    <hyperlink ref="G30" r:id="rId58"/>
+    <hyperlink ref="C31" r:id="rId59"/>
+    <hyperlink ref="G31" r:id="rId60"/>
+    <hyperlink ref="C32" r:id="rId61"/>
+    <hyperlink ref="G32" r:id="rId62"/>
+    <hyperlink ref="C33" r:id="rId63"/>
+    <hyperlink ref="G33" r:id="rId64"/>
+    <hyperlink ref="C34" r:id="rId65"/>
+    <hyperlink ref="G34" r:id="rId66"/>
+    <hyperlink ref="C35" r:id="rId67"/>
+    <hyperlink ref="G35" r:id="rId68"/>
+    <hyperlink ref="C36" r:id="rId69"/>
+    <hyperlink ref="G36" r:id="rId70"/>
+    <hyperlink ref="C37" r:id="rId71"/>
+    <hyperlink ref="G37" r:id="rId72"/>
+    <hyperlink ref="C38" r:id="rId73"/>
+    <hyperlink ref="G38" r:id="rId74"/>
+    <hyperlink ref="C39" r:id="rId75"/>
+    <hyperlink ref="G39" r:id="rId76"/>
+    <hyperlink ref="C40" r:id="rId77"/>
+    <hyperlink ref="G40" r:id="rId78"/>
+    <hyperlink ref="C41" r:id="rId79"/>
+    <hyperlink ref="G41" r:id="rId80"/>
+    <hyperlink ref="C42" r:id="rId81"/>
+    <hyperlink ref="G42" r:id="rId82"/>
+    <hyperlink ref="C43" r:id="rId83"/>
+    <hyperlink ref="G43" r:id="rId84"/>
+    <hyperlink ref="C44" r:id="rId85"/>
+    <hyperlink ref="G44" r:id="rId86"/>
+    <hyperlink ref="C45" r:id="rId87"/>
+    <hyperlink ref="G45" r:id="rId88"/>
+    <hyperlink ref="C46" r:id="rId89"/>
+    <hyperlink ref="G46" r:id="rId90"/>
+    <hyperlink ref="C47" r:id="rId91"/>
+    <hyperlink ref="G47" r:id="rId92"/>
+    <hyperlink ref="C48" r:id="rId93"/>
+    <hyperlink ref="G48" r:id="rId94"/>
+    <hyperlink ref="C49" r:id="rId95"/>
+    <hyperlink ref="G49" r:id="rId96"/>
+    <hyperlink ref="C50" r:id="rId97"/>
+    <hyperlink ref="G50" r:id="rId98"/>
+    <hyperlink ref="C51" r:id="rId99"/>
+    <hyperlink ref="G51" r:id="rId100"/>
+    <hyperlink ref="C52" r:id="rId101"/>
+    <hyperlink ref="G52" r:id="rId102"/>
+    <hyperlink ref="C53" r:id="rId103"/>
+    <hyperlink ref="G53" r:id="rId104"/>
+    <hyperlink ref="C54" r:id="rId105"/>
+    <hyperlink ref="G54" r:id="rId106"/>
+    <hyperlink ref="C55" r:id="rId107"/>
+    <hyperlink ref="G55" r:id="rId108"/>
+    <hyperlink ref="C56" r:id="rId109"/>
+    <hyperlink ref="G56" r:id="rId110"/>
+    <hyperlink ref="C57" r:id="rId111"/>
+    <hyperlink ref="G57" r:id="rId112"/>
   </hyperlinks>
-  <drawing r:id="rId114"/>
-  <legacyDrawing r:id="rId115"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId113"/>
+  <legacyDrawing r:id="rId114"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="15.13" defaultRowHeight="15.0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="15.140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="28.75"/>
-    <col customWidth="1" min="2" max="2" width="33.0"/>
-    <col customWidth="1" min="3" max="3" width="23.38"/>
-    <col customWidth="1" min="4" max="4" width="17.88"/>
-    <col customWidth="1" min="5" max="5" width="50.63"/>
+    <col min="1" max="1" width="28.7109375" customWidth="1"/>
+    <col min="2" max="2" width="33" customWidth="1"/>
+    <col min="3" max="3" width="23.42578125" customWidth="1"/>
+    <col min="4" max="4" width="17.85546875" customWidth="1"/>
+    <col min="5" max="5" width="50.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:5">
       <c r="A1" s="21" t="s">
         <v>58</v>
       </c>
@@ -5676,7 +6064,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:5">
       <c r="A2" s="29" t="s">
         <v>75</v>
       </c>
@@ -5693,7 +6081,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:5">
       <c r="A3" s="29" t="s">
         <v>75</v>
       </c>
@@ -5710,7 +6098,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:5">
       <c r="A4" s="29" t="s">
         <v>75</v>
       </c>
@@ -5727,7 +6115,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:5">
       <c r="A5" s="29" t="s">
         <v>75</v>
       </c>
@@ -5744,7 +6132,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:5">
       <c r="A6" s="29" t="s">
         <v>75</v>
       </c>
@@ -5761,7 +6149,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:5">
       <c r="A7" s="29" t="s">
         <v>75</v>
       </c>
@@ -5778,7 +6166,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:5">
       <c r="A8" s="29" t="s">
         <v>75</v>
       </c>
@@ -5795,7 +6183,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:5">
       <c r="A9" s="29" t="s">
         <v>75</v>
       </c>
@@ -5812,7 +6200,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:5">
       <c r="A10" s="29" t="s">
         <v>75</v>
       </c>
@@ -5829,7 +6217,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:5">
       <c r="A11" s="29" t="s">
         <v>75</v>
       </c>
@@ -5846,7 +6234,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:5">
       <c r="A12" s="29" t="s">
         <v>75</v>
       </c>
@@ -5863,7 +6251,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:5">
       <c r="A13" s="29" t="s">
         <v>75</v>
       </c>
@@ -5880,7 +6268,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:5">
       <c r="A14" s="29" t="s">
         <v>75</v>
       </c>
@@ -5897,7 +6285,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:5">
       <c r="A15" s="29" t="s">
         <v>75</v>
       </c>
@@ -5914,7 +6302,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:5">
       <c r="A16" s="29" t="s">
         <v>75</v>
       </c>
@@ -5931,7 +6319,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:5">
       <c r="A17" s="29" t="s">
         <v>75</v>
       </c>
@@ -5948,7 +6336,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:5">
       <c r="A18" s="29" t="s">
         <v>75</v>
       </c>
@@ -5965,7 +6353,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:5">
       <c r="A19" s="22" t="s">
         <v>162</v>
       </c>
@@ -5982,7 +6370,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:5">
       <c r="A20" s="22" t="s">
         <v>162</v>
       </c>
@@ -5999,7 +6387,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:5">
       <c r="A21" s="22" t="s">
         <v>162</v>
       </c>
@@ -6016,7 +6404,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:5">
       <c r="A22" s="22" t="s">
         <v>162</v>
       </c>
@@ -6033,7 +6421,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="1:5">
       <c r="A23" s="22" t="s">
         <v>162</v>
       </c>
@@ -6050,7 +6438,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="1:5">
       <c r="A24" s="22" t="s">
         <v>162</v>
       </c>
@@ -6067,7 +6455,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="1:5">
       <c r="A25" s="22" t="s">
         <v>162</v>
       </c>
@@ -6084,7 +6472,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" spans="1:5">
       <c r="A26" s="22" t="s">
         <v>162</v>
       </c>
@@ -6101,7 +6489,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" spans="1:5">
       <c r="A27" s="22" t="s">
         <v>162</v>
       </c>
@@ -6118,7 +6506,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" spans="1:5">
       <c r="A28" s="22" t="s">
         <v>162</v>
       </c>
@@ -6135,7 +6523,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" spans="1:5">
       <c r="A29" s="22" t="s">
         <v>162</v>
       </c>
@@ -6152,7 +6540,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" spans="1:5">
       <c r="A30" s="22" t="s">
         <v>162</v>
       </c>
@@ -6169,7 +6557,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" spans="1:5">
       <c r="A31" s="22" t="s">
         <v>162</v>
       </c>
@@ -6186,7 +6574,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="32">
+    <row r="32" spans="1:5">
       <c r="A32" s="22" t="s">
         <v>162</v>
       </c>
@@ -6203,7 +6591,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="33">
+    <row r="33" spans="1:5">
       <c r="A33" s="22" t="s">
         <v>162</v>
       </c>
@@ -6220,7 +6608,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="34">
+    <row r="34" spans="1:5">
       <c r="A34" s="22" t="s">
         <v>162</v>
       </c>
@@ -6237,7 +6625,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="35">
+    <row r="35" spans="1:5">
       <c r="A35" s="22" t="s">
         <v>162</v>
       </c>
@@ -6254,7 +6642,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="36">
+    <row r="36" spans="1:5">
       <c r="A36" s="22" t="s">
         <v>162</v>
       </c>
@@ -6271,7 +6659,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="37">
+    <row r="37" spans="1:5">
       <c r="A37" s="29" t="s">
         <v>87</v>
       </c>
@@ -6288,7 +6676,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="38">
+    <row r="38" spans="1:5">
       <c r="A38" s="29" t="s">
         <v>87</v>
       </c>
@@ -6305,7 +6693,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="39">
+    <row r="39" spans="1:5">
       <c r="A39" s="29" t="s">
         <v>87</v>
       </c>
@@ -6322,7 +6710,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="40">
+    <row r="40" spans="1:5">
       <c r="A40" s="29" t="s">
         <v>87</v>
       </c>
@@ -6339,7 +6727,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="41">
+    <row r="41" spans="1:5">
       <c r="A41" s="29" t="s">
         <v>87</v>
       </c>
@@ -6356,7 +6744,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="42">
+    <row r="42" spans="1:5">
       <c r="A42" s="29" t="s">
         <v>87</v>
       </c>
@@ -6373,7 +6761,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="43">
+    <row r="43" spans="1:5">
       <c r="A43" s="29" t="s">
         <v>87</v>
       </c>
@@ -6390,7 +6778,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="44">
+    <row r="44" spans="1:5">
       <c r="A44" s="29" t="s">
         <v>87</v>
       </c>
@@ -6407,7 +6795,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="45">
+    <row r="45" spans="1:5">
       <c r="A45" s="10" t="s">
         <v>330</v>
       </c>
@@ -6424,7 +6812,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="46">
+    <row r="46" spans="1:5">
       <c r="A46" s="10" t="s">
         <v>98</v>
       </c>
@@ -6441,7 +6829,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="47">
+    <row r="47" spans="1:5">
       <c r="A47" s="10" t="s">
         <v>98</v>
       </c>
@@ -6458,7 +6846,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="48">
+    <row r="48" spans="1:5">
       <c r="A48" s="10" t="s">
         <v>98</v>
       </c>
@@ -6475,7 +6863,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="49">
+    <row r="49" spans="1:5">
       <c r="A49" s="10" t="s">
         <v>98</v>
       </c>
@@ -6492,7 +6880,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="50">
+    <row r="50" spans="1:5">
       <c r="A50" s="10" t="s">
         <v>98</v>
       </c>
@@ -6509,7 +6897,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="51">
+    <row r="51" spans="1:5">
       <c r="A51" s="10" t="s">
         <v>98</v>
       </c>
@@ -6526,7 +6914,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="52">
+    <row r="52" spans="1:5">
       <c r="A52" s="10" t="s">
         <v>98</v>
       </c>
@@ -6543,7 +6931,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="53">
+    <row r="53" spans="1:5">
       <c r="A53" s="10" t="s">
         <v>98</v>
       </c>
@@ -6560,7 +6948,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="54">
+    <row r="54" spans="1:5">
       <c r="A54" s="10" t="s">
         <v>98</v>
       </c>
@@ -6577,52 +6965,54 @@
         <v>384</v>
       </c>
     </row>
-    <row r="55">
+    <row r="55" spans="1:5">
       <c r="A55" s="3"/>
       <c r="B55" s="35"/>
     </row>
-    <row r="56">
+    <row r="56" spans="1:5">
       <c r="A56" s="3"/>
       <c r="B56" s="35"/>
     </row>
-    <row r="57">
+    <row r="57" spans="1:5">
       <c r="A57" s="3"/>
     </row>
-    <row r="58">
+    <row r="58" spans="1:5">
       <c r="A58" s="3"/>
     </row>
   </sheetData>
-  <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="15.13" defaultRowHeight="15.0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="15.140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="2" max="2" width="20.88"/>
+    <col min="2" max="2" width="20.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:2">
       <c r="A1" s="3" t="s">
         <v>416</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:2">
       <c r="A2" s="3" t="s">
         <v>417</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:2">
       <c r="A4" s="3" t="s">
         <v>418</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:2">
       <c r="A5" s="3" t="s">
         <v>419</v>
       </c>
@@ -6630,7 +7020,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:2">
       <c r="A6" s="3" t="s">
         <v>421</v>
       </c>
@@ -6638,12 +7028,12 @@
         <v>422</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:2">
       <c r="A11" s="3" t="s">
         <v>423</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>